<commit_message>
Transportation scaled files to SEDS, new methodology for calculating BAADVBT
</commit_message>
<xml_diff>
--- a/InputData/trans/SYVbT/Start Year Vehicles by Technology.xlsx
+++ b/InputData/trans/SYVbT/Start Year Vehicles by Technology.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\Colorado\CO_Model\InputData\trans\SYVbT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A0F25F-C7F9-4A30-8D6B-0D62C4212CCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E05F7ED-92F7-46FB-844A-6328AAA5B800}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1845" yWindow="930" windowWidth="25035" windowHeight="15225" firstSheet="3" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11310" yWindow="2385" windowWidth="16350" windowHeight="14475" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30" yWindow="675" windowWidth="19695" windowHeight="11580" firstSheet="10" activeTab="12" xr2:uid="{D06A4721-035E-484A-B74D-F75D504BA890}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -4203,7 +4204,7 @@
     </xf>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyAlignment="1">
@@ -4373,34 +4374,55 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -4410,42 +4432,22 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
+    <xf numFmtId="170" fontId="8" fillId="0" borderId="0" xfId="142" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="143">
     <cellStyle name="20% - Accent1 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
@@ -5012,6 +5014,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A53" sqref="A53:A55"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
@@ -5375,6 +5378,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
@@ -5613,6 +5617,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
@@ -5701,6 +5706,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
@@ -6072,8 +6078,14 @@
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
+  <cols>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="61" t="s">
@@ -6282,7 +6294,7 @@
       <c r="D12">
         <v>8971212.6459999997</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="100">
         <v>4869416.5039999997</v>
       </c>
       <c r="F12">
@@ -6305,7 +6317,7 @@
       <c r="D13">
         <v>2586744</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="100">
         <v>9405890</v>
       </c>
       <c r="F13">
@@ -6419,9 +6431,10 @@
   </sheetPr>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
@@ -6654,8 +6667,11 @@
   </sheetPr>
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -6709,12 +6725,11 @@
         <v>196</v>
       </c>
       <c r="D2" s="18">
-        <f>ROUND('USA Values'!D12*'Share of VT by state'!$B$4,0)</f>
-        <v>151641</v>
+        <f>SUM(ROUND('USA Values'!D12*'Share of VT by state'!$B$4,0),ROUND('USA Values'!D13*'Share of VT by state'!$B$5,0))</f>
+        <v>195365</v>
       </c>
       <c r="E2" s="18">
-        <f>ROUND('USA Values'!E12*'Share of VT by state'!$B$4,0)</f>
-        <v>82308</v>
+        <v>0</v>
       </c>
       <c r="F2" s="18">
         <f>ROUND('USA Values'!F12*'Share of VT by state'!$B$4,0)</f>
@@ -6744,12 +6759,11 @@
         <v>626</v>
       </c>
       <c r="D3">
-        <f>ROUND('USA Values'!D13*'Share of VT by state'!$B$5,0)</f>
-        <v>43724</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <f>ROUND('USA Values'!E13*'Share of VT by state'!$B$5,0)</f>
-        <v>158989</v>
+        <f>SUM(ROUND('USA Values'!E13*'Share of VT by state'!$B$5,0),ROUND('USA Values'!E12*'Share of VT by state'!$B$4,0))</f>
+        <v>241297</v>
       </c>
       <c r="F3">
         <f>ROUND('USA Values'!F13*'Share of VT by state'!$B$5,0)</f>
@@ -6888,6 +6902,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
   <cols>
@@ -6946,6 +6961,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
+    <sheetView topLeftCell="B1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -13710,6 +13726,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
+    <sheetView topLeftCell="B1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -24335,6 +24352,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
+    <sheetView topLeftCell="B1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -29197,6 +29215,7 @@
   <dimension ref="A1:AJ87"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
@@ -35042,6 +35061,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
+    <sheetView topLeftCell="B1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -54993,6 +55013,7 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
+    <sheetView topLeftCell="B1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -79778,6 +79799,9 @@
     <sheetView workbookViewId="0">
       <selection activeCell="AK31" sqref="AK31"/>
     </sheetView>
+    <sheetView workbookViewId="1">
+      <selection sqref="A1:AI1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
@@ -79792,43 +79816,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="91" t="s">
         <v>928</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
-      <c r="K1" s="85"/>
-      <c r="L1" s="85"/>
-      <c r="M1" s="85"/>
-      <c r="N1" s="85"/>
-      <c r="O1" s="85"/>
-      <c r="P1" s="85"/>
-      <c r="Q1" s="85"/>
-      <c r="R1" s="85"/>
-      <c r="S1" s="85"/>
-      <c r="T1" s="85"/>
-      <c r="U1" s="85"/>
-      <c r="V1" s="85"/>
-      <c r="W1" s="85"/>
-      <c r="X1" s="85"/>
-      <c r="Y1" s="85"/>
-      <c r="Z1" s="85"/>
-      <c r="AA1" s="85"/>
-      <c r="AB1" s="85"/>
-      <c r="AC1" s="85"/>
-      <c r="AD1" s="85"/>
-      <c r="AE1" s="85"/>
-      <c r="AF1" s="85"/>
-      <c r="AG1" s="85"/>
-      <c r="AH1" s="85"/>
-      <c r="AI1" s="85"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="92"/>
+      <c r="G1" s="92"/>
+      <c r="H1" s="92"/>
+      <c r="I1" s="92"/>
+      <c r="J1" s="92"/>
+      <c r="K1" s="92"/>
+      <c r="L1" s="92"/>
+      <c r="M1" s="92"/>
+      <c r="N1" s="92"/>
+      <c r="O1" s="92"/>
+      <c r="P1" s="92"/>
+      <c r="Q1" s="92"/>
+      <c r="R1" s="92"/>
+      <c r="S1" s="92"/>
+      <c r="T1" s="92"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="92"/>
+      <c r="W1" s="92"/>
+      <c r="X1" s="92"/>
+      <c r="Y1" s="92"/>
+      <c r="Z1" s="92"/>
+      <c r="AA1" s="92"/>
+      <c r="AB1" s="92"/>
+      <c r="AC1" s="92"/>
+      <c r="AD1" s="92"/>
+      <c r="AE1" s="92"/>
+      <c r="AF1" s="92"/>
+      <c r="AG1" s="92"/>
+      <c r="AH1" s="92"/>
+      <c r="AI1" s="92"/>
     </row>
     <row r="2" spans="1:37" s="19" customFormat="1" ht="16.5" customHeight="1">
       <c r="A2" s="31"/>
@@ -83092,26 +83116,26 @@
       </c>
     </row>
     <row r="35" spans="1:35" s="70" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A35" s="86" t="s">
+      <c r="A35" s="93" t="s">
         <v>963</v>
       </c>
-      <c r="B35" s="87"/>
-      <c r="C35" s="87"/>
-      <c r="D35" s="87"/>
-      <c r="E35" s="87"/>
-      <c r="F35" s="87"/>
-      <c r="G35" s="87"/>
-      <c r="H35" s="87"/>
-      <c r="I35" s="87"/>
-      <c r="J35" s="87"/>
-      <c r="K35" s="87"/>
-      <c r="L35" s="87"/>
-      <c r="M35" s="87"/>
-      <c r="N35" s="87"/>
-      <c r="O35" s="87"/>
-      <c r="P35" s="87"/>
-      <c r="Q35" s="87"/>
-      <c r="R35" s="87"/>
+      <c r="B35" s="94"/>
+      <c r="C35" s="94"/>
+      <c r="D35" s="94"/>
+      <c r="E35" s="94"/>
+      <c r="F35" s="94"/>
+      <c r="G35" s="94"/>
+      <c r="H35" s="94"/>
+      <c r="I35" s="94"/>
+      <c r="J35" s="94"/>
+      <c r="K35" s="94"/>
+      <c r="L35" s="94"/>
+      <c r="M35" s="94"/>
+      <c r="N35" s="94"/>
+      <c r="O35" s="94"/>
+      <c r="P35" s="94"/>
+      <c r="Q35" s="94"/>
+      <c r="R35" s="94"/>
       <c r="S35" s="54"/>
       <c r="T35" s="54"/>
       <c r="U35" s="54"/>
@@ -83127,26 +83151,26 @@
     </row>
     <row r="36" spans="1:35" s="70" customFormat="1" ht="12.75" customHeight="1">
       <c r="A36" s="88"/>
-      <c r="B36" s="89"/>
-      <c r="C36" s="89"/>
-      <c r="D36" s="89"/>
-      <c r="E36" s="89"/>
-      <c r="F36" s="89"/>
-      <c r="G36" s="89"/>
-      <c r="H36" s="89"/>
-      <c r="I36" s="89"/>
-      <c r="J36" s="89"/>
-      <c r="K36" s="89"/>
-      <c r="L36" s="89"/>
-      <c r="M36" s="89"/>
-      <c r="N36" s="89"/>
-      <c r="O36" s="89"/>
-      <c r="P36" s="89"/>
-      <c r="Q36" s="89"/>
-      <c r="R36" s="89"/>
+      <c r="B36" s="95"/>
+      <c r="C36" s="95"/>
+      <c r="D36" s="95"/>
+      <c r="E36" s="95"/>
+      <c r="F36" s="95"/>
+      <c r="G36" s="95"/>
+      <c r="H36" s="95"/>
+      <c r="I36" s="95"/>
+      <c r="J36" s="95"/>
+      <c r="K36" s="95"/>
+      <c r="L36" s="95"/>
+      <c r="M36" s="95"/>
+      <c r="N36" s="95"/>
+      <c r="O36" s="95"/>
+      <c r="P36" s="95"/>
+      <c r="Q36" s="95"/>
+      <c r="R36" s="95"/>
     </row>
     <row r="37" spans="1:35" s="68" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A37" s="90" t="s">
+      <c r="A37" s="96" t="s">
         <v>964</v>
       </c>
       <c r="B37" s="75"/>
@@ -83168,7 +83192,7 @@
       <c r="R37" s="75"/>
     </row>
     <row r="38" spans="1:35" s="68" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A38" s="83" t="s">
+      <c r="A38" s="74" t="s">
         <v>965</v>
       </c>
       <c r="B38" s="75"/>
@@ -83190,7 +83214,7 @@
       <c r="R38" s="75"/>
     </row>
     <row r="39" spans="1:35" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A39" s="74" t="s">
+      <c r="A39" s="76" t="s">
         <v>966</v>
       </c>
       <c r="B39" s="75"/>
@@ -83212,7 +83236,7 @@
       <c r="R39" s="75"/>
     </row>
     <row r="40" spans="1:35" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A40" s="83" t="s">
+      <c r="A40" s="74" t="s">
         <v>967</v>
       </c>
       <c r="B40" s="75"/>
@@ -83234,7 +83258,7 @@
       <c r="R40" s="75"/>
     </row>
     <row r="41" spans="1:35" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A41" s="83" t="s">
+      <c r="A41" s="74" t="s">
         <v>968</v>
       </c>
       <c r="B41" s="75"/>
@@ -83256,7 +83280,7 @@
       <c r="R41" s="75"/>
     </row>
     <row r="42" spans="1:35" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A42" s="83" t="s">
+      <c r="A42" s="74" t="s">
         <v>969</v>
       </c>
       <c r="B42" s="75"/>
@@ -83278,7 +83302,7 @@
       <c r="R42" s="75"/>
     </row>
     <row r="43" spans="1:35" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A43" s="74" t="s">
+      <c r="A43" s="76" t="s">
         <v>970</v>
       </c>
       <c r="B43" s="75"/>
@@ -83300,7 +83324,7 @@
       <c r="R43" s="75"/>
     </row>
     <row r="44" spans="1:35" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A44" s="74" t="s">
+      <c r="A44" s="76" t="s">
         <v>971</v>
       </c>
       <c r="B44" s="75"/>
@@ -83322,7 +83346,7 @@
       <c r="R44" s="75"/>
     </row>
     <row r="45" spans="1:35" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A45" s="95" t="s">
+      <c r="A45" s="77" t="s">
         <v>972</v>
       </c>
       <c r="B45" s="75"/>
@@ -83344,7 +83368,7 @@
       <c r="R45" s="75"/>
     </row>
     <row r="46" spans="1:35" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A46" s="83" t="s">
+      <c r="A46" s="74" t="s">
         <v>973</v>
       </c>
       <c r="B46" s="75"/>
@@ -83366,7 +83390,7 @@
       <c r="R46" s="75"/>
     </row>
     <row r="47" spans="1:35" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A47" s="83" t="s">
+      <c r="A47" s="74" t="s">
         <v>974</v>
       </c>
       <c r="B47" s="75"/>
@@ -83388,7 +83412,7 @@
       <c r="R47" s="75"/>
     </row>
     <row r="48" spans="1:35" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A48" s="83" t="s">
+      <c r="A48" s="74" t="s">
         <v>975</v>
       </c>
       <c r="B48" s="75"/>
@@ -83410,7 +83434,7 @@
       <c r="R48" s="75"/>
     </row>
     <row r="49" spans="1:18" s="68" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A49" s="83" t="s">
+      <c r="A49" s="74" t="s">
         <v>976</v>
       </c>
       <c r="B49" s="75"/>
@@ -83432,7 +83456,7 @@
       <c r="R49" s="75"/>
     </row>
     <row r="50" spans="1:18" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A50" s="83" t="s">
+      <c r="A50" s="74" t="s">
         <v>977</v>
       </c>
       <c r="B50" s="75"/>
@@ -83452,7 +83476,7 @@
       <c r="P50" s="75"/>
     </row>
     <row r="51" spans="1:18" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A51" s="76"/>
+      <c r="A51" s="97"/>
       <c r="B51" s="75"/>
       <c r="C51" s="75"/>
       <c r="D51" s="75"/>
@@ -83470,7 +83494,7 @@
       <c r="P51" s="75"/>
     </row>
     <row r="52" spans="1:18" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A52" s="94" t="s">
+      <c r="A52" s="86" t="s">
         <v>978</v>
       </c>
       <c r="B52" s="75"/>
@@ -83490,7 +83514,7 @@
       <c r="P52" s="75"/>
     </row>
     <row r="53" spans="1:18" s="68" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A53" s="95" t="s">
+      <c r="A53" s="77" t="s">
         <v>979</v>
       </c>
       <c r="B53" s="75"/>
@@ -83510,7 +83534,7 @@
       <c r="P53" s="75"/>
     </row>
     <row r="54" spans="1:18" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A54" s="77" t="s">
+      <c r="A54" s="79" t="s">
         <v>980</v>
       </c>
       <c r="B54" s="75"/>
@@ -83530,7 +83554,7 @@
       <c r="P54" s="75"/>
     </row>
     <row r="55" spans="1:18" s="68" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A55" s="79" t="s">
+      <c r="A55" s="98" t="s">
         <v>981</v>
       </c>
       <c r="B55" s="75"/>
@@ -83550,7 +83574,7 @@
       <c r="P55" s="75"/>
     </row>
     <row r="56" spans="1:18" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A56" s="77" t="s">
+      <c r="A56" s="79" t="s">
         <v>982</v>
       </c>
       <c r="B56" s="75"/>
@@ -83570,7 +83594,7 @@
       <c r="P56" s="75"/>
     </row>
     <row r="57" spans="1:18" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A57" s="77" t="s">
+      <c r="A57" s="79" t="s">
         <v>983</v>
       </c>
       <c r="B57" s="75"/>
@@ -83590,7 +83614,7 @@
       <c r="P57" s="75"/>
     </row>
     <row r="58" spans="1:18" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A58" s="96" t="s">
+      <c r="A58" s="87" t="s">
         <v>984</v>
       </c>
       <c r="B58" s="75"/>
@@ -83610,7 +83634,7 @@
       <c r="P58" s="75"/>
     </row>
     <row r="59" spans="1:18" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A59" s="81"/>
+      <c r="A59" s="99"/>
       <c r="B59" s="75"/>
       <c r="C59" s="75"/>
       <c r="D59" s="75"/>
@@ -83688,7 +83712,7 @@
       <c r="P62" s="75"/>
     </row>
     <row r="63" spans="1:18" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A63" s="97" t="s">
+      <c r="A63" s="89" t="s">
         <v>988</v>
       </c>
       <c r="B63" s="75"/>
@@ -83908,7 +83932,7 @@
       <c r="P73" s="75"/>
     </row>
     <row r="74" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A74" s="80" t="s">
+      <c r="A74" s="84" t="s">
         <v>999</v>
       </c>
       <c r="B74" s="75"/>
@@ -83948,7 +83972,7 @@
       <c r="P75" s="75"/>
     </row>
     <row r="76" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A76" s="77" t="s">
+      <c r="A76" s="79" t="s">
         <v>1001</v>
       </c>
       <c r="B76" s="75"/>
@@ -83968,7 +83992,7 @@
       <c r="P76" s="75"/>
     </row>
     <row r="77" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A77" s="93" t="s">
+      <c r="A77" s="83" t="s">
         <v>1002</v>
       </c>
       <c r="B77" s="75"/>
@@ -83988,7 +84012,7 @@
       <c r="P77" s="75"/>
     </row>
     <row r="78" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A78" s="92" t="s">
+      <c r="A78" s="85" t="s">
         <v>1003</v>
       </c>
       <c r="B78" s="75"/>
@@ -84008,7 +84032,7 @@
       <c r="P78" s="75"/>
     </row>
     <row r="79" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A79" s="93" t="s">
+      <c r="A79" s="83" t="s">
         <v>1004</v>
       </c>
       <c r="B79" s="75"/>
@@ -84048,7 +84072,7 @@
       <c r="P80" s="75"/>
     </row>
     <row r="81" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A81" s="77" t="s">
+      <c r="A81" s="79" t="s">
         <v>1006</v>
       </c>
       <c r="B81" s="75"/>
@@ -84068,7 +84092,7 @@
       <c r="P81" s="75"/>
     </row>
     <row r="82" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A82" s="93" t="s">
+      <c r="A82" s="83" t="s">
         <v>1007</v>
       </c>
       <c r="B82" s="75"/>
@@ -84108,7 +84132,7 @@
       <c r="P83" s="75"/>
     </row>
     <row r="84" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A84" s="77" t="s">
+      <c r="A84" s="79" t="s">
         <v>1009</v>
       </c>
       <c r="B84" s="75"/>
@@ -84128,7 +84152,7 @@
       <c r="P84" s="75"/>
     </row>
     <row r="85" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A85" s="93" t="s">
+      <c r="A85" s="83" t="s">
         <v>1002</v>
       </c>
       <c r="B85" s="75"/>
@@ -84148,7 +84172,7 @@
       <c r="P85" s="75"/>
     </row>
     <row r="86" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A86" s="92" t="s">
+      <c r="A86" s="85" t="s">
         <v>1010</v>
       </c>
       <c r="B86" s="75"/>
@@ -84168,7 +84192,7 @@
       <c r="P86" s="75"/>
     </row>
     <row r="87" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A87" s="93" t="s">
+      <c r="A87" s="83" t="s">
         <v>1004</v>
       </c>
       <c r="B87" s="75"/>
@@ -84208,7 +84232,7 @@
       <c r="P88" s="75"/>
     </row>
     <row r="89" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A89" s="77" t="s">
+      <c r="A89" s="79" t="s">
         <v>1012</v>
       </c>
       <c r="B89" s="75"/>
@@ -84228,7 +84252,7 @@
       <c r="P89" s="75"/>
     </row>
     <row r="90" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A90" s="93" t="s">
+      <c r="A90" s="83" t="s">
         <v>1007</v>
       </c>
       <c r="B90" s="75"/>
@@ -84248,7 +84272,7 @@
       <c r="P90" s="75"/>
     </row>
     <row r="91" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A91" s="80" t="s">
+      <c r="A91" s="84" t="s">
         <v>1013</v>
       </c>
       <c r="B91" s="75"/>
@@ -84328,7 +84352,7 @@
       <c r="P94" s="75"/>
     </row>
     <row r="95" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A95" s="80" t="s">
+      <c r="A95" s="84" t="s">
         <v>1017</v>
       </c>
       <c r="B95" s="75"/>
@@ -84371,24 +84395,24 @@
       <c r="A97" s="78" t="s">
         <v>1018</v>
       </c>
-      <c r="B97" s="91"/>
-      <c r="C97" s="91"/>
-      <c r="D97" s="91"/>
-      <c r="E97" s="91"/>
-      <c r="F97" s="91"/>
-      <c r="G97" s="91"/>
-      <c r="H97" s="91"/>
-      <c r="I97" s="91"/>
-      <c r="J97" s="91"/>
-      <c r="K97" s="91"/>
-      <c r="L97" s="91"/>
-      <c r="M97" s="91"/>
-      <c r="N97" s="91"/>
-      <c r="O97" s="91"/>
-      <c r="P97" s="91"/>
+      <c r="B97" s="90"/>
+      <c r="C97" s="90"/>
+      <c r="D97" s="90"/>
+      <c r="E97" s="90"/>
+      <c r="F97" s="90"/>
+      <c r="G97" s="90"/>
+      <c r="H97" s="90"/>
+      <c r="I97" s="90"/>
+      <c r="J97" s="90"/>
+      <c r="K97" s="90"/>
+      <c r="L97" s="90"/>
+      <c r="M97" s="90"/>
+      <c r="N97" s="90"/>
+      <c r="O97" s="90"/>
+      <c r="P97" s="90"/>
     </row>
     <row r="98" spans="1:20" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A98" s="80" t="s">
+      <c r="A98" s="84" t="s">
         <v>1019</v>
       </c>
       <c r="B98" s="75"/>
@@ -84488,7 +84512,7 @@
       <c r="P102" s="75"/>
     </row>
     <row r="103" spans="1:20" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A103" s="80" t="s">
+      <c r="A103" s="84" t="s">
         <v>1024</v>
       </c>
       <c r="B103" s="75"/>
@@ -84528,7 +84552,7 @@
       <c r="P104" s="75"/>
     </row>
     <row r="105" spans="1:20" s="68" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A105" s="77" t="s">
+      <c r="A105" s="79" t="s">
         <v>1026</v>
       </c>
       <c r="B105" s="75"/>
@@ -84548,7 +84572,7 @@
       <c r="P105" s="75"/>
     </row>
     <row r="106" spans="1:20" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A106" s="77" t="s">
+      <c r="A106" s="79" t="s">
         <v>1027</v>
       </c>
       <c r="B106" s="75"/>
@@ -84588,7 +84612,7 @@
       <c r="P107" s="75"/>
     </row>
     <row r="108" spans="1:20" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A108" s="98" t="s">
+      <c r="A108" s="80" t="s">
         <v>1029</v>
       </c>
       <c r="B108" s="75"/>
@@ -84608,7 +84632,7 @@
       <c r="P108" s="75"/>
     </row>
     <row r="109" spans="1:20" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A109" s="99" t="s">
+      <c r="A109" s="81" t="s">
         <v>1030</v>
       </c>
       <c r="B109" s="75"/>
@@ -84725,15 +84749,59 @@
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="A46:R46"/>
-    <mergeCell ref="A47:R47"/>
-    <mergeCell ref="A48:R48"/>
-    <mergeCell ref="A49:R49"/>
-    <mergeCell ref="A41:R41"/>
-    <mergeCell ref="A42:R42"/>
-    <mergeCell ref="A43:R43"/>
-    <mergeCell ref="A44:R44"/>
-    <mergeCell ref="A45:R45"/>
+    <mergeCell ref="A39:R39"/>
+    <mergeCell ref="A51:P51"/>
+    <mergeCell ref="A76:P76"/>
+    <mergeCell ref="A70:P70"/>
+    <mergeCell ref="A65:P65"/>
+    <mergeCell ref="A55:P55"/>
+    <mergeCell ref="A56:P56"/>
+    <mergeCell ref="A57:P57"/>
+    <mergeCell ref="A71:P71"/>
+    <mergeCell ref="A72:P72"/>
+    <mergeCell ref="A73:P73"/>
+    <mergeCell ref="A74:P74"/>
+    <mergeCell ref="A69:P69"/>
+    <mergeCell ref="A59:P59"/>
+    <mergeCell ref="A75:P75"/>
+    <mergeCell ref="A40:R40"/>
+    <mergeCell ref="A1:AI1"/>
+    <mergeCell ref="A35:R35"/>
+    <mergeCell ref="A36:R36"/>
+    <mergeCell ref="A37:R37"/>
+    <mergeCell ref="A38:R38"/>
+    <mergeCell ref="A107:P107"/>
+    <mergeCell ref="A100:P100"/>
+    <mergeCell ref="A97:P97"/>
+    <mergeCell ref="A99:P99"/>
+    <mergeCell ref="A96:P96"/>
+    <mergeCell ref="A98:P98"/>
+    <mergeCell ref="A101:P101"/>
+    <mergeCell ref="A78:P78"/>
+    <mergeCell ref="A79:P79"/>
+    <mergeCell ref="A80:P80"/>
+    <mergeCell ref="A52:P52"/>
+    <mergeCell ref="A53:P53"/>
+    <mergeCell ref="A58:P58"/>
+    <mergeCell ref="A54:P54"/>
+    <mergeCell ref="A77:P77"/>
+    <mergeCell ref="A60:P60"/>
+    <mergeCell ref="A61:P61"/>
+    <mergeCell ref="A62:P62"/>
+    <mergeCell ref="A63:P63"/>
+    <mergeCell ref="A64:P64"/>
+    <mergeCell ref="A66:P66"/>
+    <mergeCell ref="A67:P67"/>
+    <mergeCell ref="A68:P68"/>
+    <mergeCell ref="A89:P89"/>
+    <mergeCell ref="A90:P90"/>
+    <mergeCell ref="A95:P95"/>
+    <mergeCell ref="A81:P81"/>
+    <mergeCell ref="A82:P82"/>
+    <mergeCell ref="A84:P84"/>
+    <mergeCell ref="A85:P85"/>
+    <mergeCell ref="A86:P86"/>
+    <mergeCell ref="A83:P83"/>
     <mergeCell ref="A111:P111"/>
     <mergeCell ref="A50:P50"/>
     <mergeCell ref="A92:P92"/>
@@ -84750,59 +84818,15 @@
     <mergeCell ref="A103:P103"/>
     <mergeCell ref="A104:P104"/>
     <mergeCell ref="A91:P91"/>
-    <mergeCell ref="A89:P89"/>
-    <mergeCell ref="A90:P90"/>
-    <mergeCell ref="A95:P95"/>
-    <mergeCell ref="A81:P81"/>
-    <mergeCell ref="A82:P82"/>
-    <mergeCell ref="A84:P84"/>
-    <mergeCell ref="A85:P85"/>
-    <mergeCell ref="A86:P86"/>
-    <mergeCell ref="A83:P83"/>
-    <mergeCell ref="A78:P78"/>
-    <mergeCell ref="A79:P79"/>
-    <mergeCell ref="A80:P80"/>
-    <mergeCell ref="A52:P52"/>
-    <mergeCell ref="A53:P53"/>
-    <mergeCell ref="A58:P58"/>
-    <mergeCell ref="A54:P54"/>
-    <mergeCell ref="A77:P77"/>
-    <mergeCell ref="A60:P60"/>
-    <mergeCell ref="A61:P61"/>
-    <mergeCell ref="A62:P62"/>
-    <mergeCell ref="A63:P63"/>
-    <mergeCell ref="A64:P64"/>
-    <mergeCell ref="A66:P66"/>
-    <mergeCell ref="A67:P67"/>
-    <mergeCell ref="A68:P68"/>
-    <mergeCell ref="A107:P107"/>
-    <mergeCell ref="A100:P100"/>
-    <mergeCell ref="A97:P97"/>
-    <mergeCell ref="A99:P99"/>
-    <mergeCell ref="A96:P96"/>
-    <mergeCell ref="A98:P98"/>
-    <mergeCell ref="A101:P101"/>
-    <mergeCell ref="A1:AI1"/>
-    <mergeCell ref="A35:R35"/>
-    <mergeCell ref="A36:R36"/>
-    <mergeCell ref="A37:R37"/>
-    <mergeCell ref="A38:R38"/>
-    <mergeCell ref="A39:R39"/>
-    <mergeCell ref="A51:P51"/>
-    <mergeCell ref="A76:P76"/>
-    <mergeCell ref="A70:P70"/>
-    <mergeCell ref="A65:P65"/>
-    <mergeCell ref="A55:P55"/>
-    <mergeCell ref="A56:P56"/>
-    <mergeCell ref="A57:P57"/>
-    <mergeCell ref="A71:P71"/>
-    <mergeCell ref="A72:P72"/>
-    <mergeCell ref="A73:P73"/>
-    <mergeCell ref="A74:P74"/>
-    <mergeCell ref="A69:P69"/>
-    <mergeCell ref="A59:P59"/>
-    <mergeCell ref="A75:P75"/>
-    <mergeCell ref="A40:R40"/>
+    <mergeCell ref="A46:R46"/>
+    <mergeCell ref="A47:R47"/>
+    <mergeCell ref="A48:R48"/>
+    <mergeCell ref="A49:R49"/>
+    <mergeCell ref="A41:R41"/>
+    <mergeCell ref="A42:R42"/>
+    <mergeCell ref="A43:R43"/>
+    <mergeCell ref="A44:R44"/>
+    <mergeCell ref="A45:R45"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="35" fitToHeight="0" orientation="landscape"/>

</xml_diff>

<commit_message>
updated transp files from jun
</commit_message>
<xml_diff>
--- a/InputData/trans/SYVbT/Start Year Vehicles by Technology.xlsx
+++ b/InputData/trans/SYVbT/Start Year Vehicles by Technology.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\Colorado\CO_Model\InputData\trans\SYVbT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/users/junshepard/library/containers/com.microsoft.excel/data/state-eps-data-repository/co/trans/syvbt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A0F25F-C7F9-4A30-8D6B-0D62C4212CCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F204CF2D-EC8C-5C48-BC1A-358DB0738733}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1845" yWindow="930" windowWidth="25035" windowHeight="15225" firstSheet="3" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="19700" windowHeight="11580" firstSheet="10" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -4203,7 +4203,7 @@
     </xf>
     <xf numFmtId="43" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="3" applyNumberFormat="1" applyAlignment="1">
@@ -4356,6 +4356,10 @@
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="142" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="170" fontId="8" fillId="0" borderId="0" xfId="142" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -4365,42 +4369,60 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="8" xfId="16" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -4410,41 +4432,20 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="143">
@@ -5009,13 +5010,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A53" sqref="A53:A55"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="73.140625" style="58" customWidth="1"/>
+    <col min="2" max="2" width="73.1640625" style="58" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -5376,15 +5375,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" style="58" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="58" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="58" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="58" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" style="58" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" style="58" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" style="58" customWidth="1"/>
+    <col min="1" max="1" width="26.83203125" style="58" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="58" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="58" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" style="58" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="58" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" style="58" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" style="58" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -5614,11 +5613,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="58" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="58" customWidth="1"/>
-    <col min="3" max="5" width="16.85546875" style="58" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" style="58" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="58" customWidth="1"/>
+    <col min="3" max="5" width="16.83203125" style="58" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -5698,14 +5697,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:AG19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.140625" style="58" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" style="58" customWidth="1"/>
+    <col min="1" max="1" width="27.1640625" style="58" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" style="58" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33">
@@ -6033,25 +6030,25 @@
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="71" t="s">
+      <c r="A18" s="68" t="s">
         <v>1068</v>
       </c>
-      <c r="B18" s="71" t="s">
+      <c r="B18" s="68" t="s">
         <v>1069</v>
       </c>
-      <c r="C18" s="71" t="s">
+      <c r="C18" s="68" t="s">
         <v>1070</v>
       </c>
-      <c r="D18" s="71" t="s">
+      <c r="D18" s="68" t="s">
         <v>1071</v>
       </c>
-      <c r="E18" s="71" t="s">
+      <c r="E18" s="68" t="s">
         <v>1072</v>
       </c>
-      <c r="F18" s="71" t="s">
+      <c r="F18" s="68" t="s">
         <v>1073</v>
       </c>
-      <c r="G18" s="71" t="s">
+      <c r="G18" s="68" t="s">
         <v>1074</v>
       </c>
     </row>
@@ -6070,17 +6067,20 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15"/>
+  <cols>
+    <col min="5" max="5" width="13.33203125" style="58" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="61" t="s">
         <v>1075</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="32.1" customHeight="1">
+    <row r="2" spans="1:7" ht="32" customHeight="1">
       <c r="A2" s="57" t="s">
         <v>1076</v>
       </c>
@@ -6282,7 +6282,7 @@
       <c r="D12">
         <v>8971212.6459999997</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="69">
         <v>4869416.5039999997</v>
       </c>
       <c r="F12">
@@ -6305,7 +6305,7 @@
       <c r="D13">
         <v>2586744</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="69">
         <v>9405890</v>
       </c>
       <c r="F13">
@@ -6420,21 +6420,21 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="58" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" style="58" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" style="58" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" style="58" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" style="58" customWidth="1"/>
-    <col min="6" max="8" width="23.28515625" style="58" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" style="58" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" style="58" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" style="58" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" style="58" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="58" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" style="58" customWidth="1"/>
+    <col min="6" max="8" width="23.33203125" style="58" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" style="58" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.95" customHeight="1">
+    <row r="1" spans="1:10" ht="16" customHeight="1">
       <c r="A1" s="57" t="s">
         <v>1076</v>
       </c>
@@ -6543,7 +6543,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="18">
-        <v>370</v>
+        <v>246</v>
       </c>
       <c r="F4" s="18">
         <v>0</v>
@@ -6655,22 +6655,22 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="58" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" style="58" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" style="58" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" style="58" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" style="58" customWidth="1"/>
-    <col min="6" max="8" width="23.28515625" style="58" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" style="58" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" style="58" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" style="58" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" style="58" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" style="58" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" style="58" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" style="58" customWidth="1"/>
+    <col min="6" max="8" width="23.33203125" style="58" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" style="58" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="58" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.95" customHeight="1">
+    <row r="1" spans="1:10" ht="16" customHeight="1">
       <c r="A1" s="57" t="s">
         <v>1076</v>
       </c>
@@ -6709,12 +6709,11 @@
         <v>196</v>
       </c>
       <c r="D2" s="18">
-        <f>ROUND('USA Values'!D12*'Share of VT by state'!$B$4,0)</f>
-        <v>151641</v>
+        <f>SUM(ROUND('USA Values'!D12*'Share of VT by state'!$B$4,0),ROUND('USA Values'!D13*'Share of VT by state'!$B$5,0))</f>
+        <v>195365</v>
       </c>
       <c r="E2" s="18">
-        <f>ROUND('USA Values'!E12*'Share of VT by state'!$B$4,0)</f>
-        <v>82308</v>
+        <v>0</v>
       </c>
       <c r="F2" s="18">
         <f>ROUND('USA Values'!F12*'Share of VT by state'!$B$4,0)</f>
@@ -6744,12 +6743,11 @@
         <v>626</v>
       </c>
       <c r="D3">
-        <f>ROUND('USA Values'!D13*'Share of VT by state'!$B$5,0)</f>
-        <v>43724</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <f>ROUND('USA Values'!E13*'Share of VT by state'!$B$5,0)</f>
-        <v>158989</v>
+        <f>SUM(ROUND('USA Values'!E13*'Share of VT by state'!$B$5,0),ROUND('USA Values'!E12*'Share of VT by state'!$B$4,0))</f>
+        <v>241297</v>
       </c>
       <c r="F3">
         <f>ROUND('USA Values'!F13*'Share of VT by state'!$B$5,0)</f>
@@ -6885,13 +6883,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" style="58" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="58" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -6940,17 +6936,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AL107"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView topLeftCell="B1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="58" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" style="58" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" style="58" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="45.6640625" style="58" customWidth="1"/>
     <col min="38" max="38" width="8" style="58" customWidth="1"/>
   </cols>
   <sheetData>
@@ -13552,44 +13543,44 @@
     </row>
     <row r="86" spans="1:37" ht="15" customHeight="1" thickBot="1"/>
     <row r="87" spans="1:37" ht="15" customHeight="1">
-      <c r="B87" s="72" t="s">
+      <c r="B87" s="73" t="s">
         <v>182</v>
       </c>
-      <c r="C87" s="73"/>
-      <c r="D87" s="73"/>
-      <c r="E87" s="73"/>
-      <c r="F87" s="73"/>
-      <c r="G87" s="73"/>
-      <c r="H87" s="73"/>
-      <c r="I87" s="73"/>
-      <c r="J87" s="73"/>
-      <c r="K87" s="73"/>
-      <c r="L87" s="73"/>
-      <c r="M87" s="73"/>
-      <c r="N87" s="73"/>
-      <c r="O87" s="73"/>
-      <c r="P87" s="73"/>
-      <c r="Q87" s="73"/>
-      <c r="R87" s="73"/>
-      <c r="S87" s="73"/>
-      <c r="T87" s="73"/>
-      <c r="U87" s="73"/>
-      <c r="V87" s="73"/>
-      <c r="W87" s="73"/>
-      <c r="X87" s="73"/>
-      <c r="Y87" s="73"/>
-      <c r="Z87" s="73"/>
-      <c r="AA87" s="73"/>
-      <c r="AB87" s="73"/>
-      <c r="AC87" s="73"/>
-      <c r="AD87" s="73"/>
-      <c r="AE87" s="73"/>
-      <c r="AF87" s="73"/>
-      <c r="AG87" s="73"/>
-      <c r="AH87" s="73"/>
-      <c r="AI87" s="73"/>
-      <c r="AJ87" s="73"/>
-      <c r="AK87" s="73"/>
+      <c r="C87" s="74"/>
+      <c r="D87" s="74"/>
+      <c r="E87" s="74"/>
+      <c r="F87" s="74"/>
+      <c r="G87" s="74"/>
+      <c r="H87" s="74"/>
+      <c r="I87" s="74"/>
+      <c r="J87" s="74"/>
+      <c r="K87" s="74"/>
+      <c r="L87" s="74"/>
+      <c r="M87" s="74"/>
+      <c r="N87" s="74"/>
+      <c r="O87" s="74"/>
+      <c r="P87" s="74"/>
+      <c r="Q87" s="74"/>
+      <c r="R87" s="74"/>
+      <c r="S87" s="74"/>
+      <c r="T87" s="74"/>
+      <c r="U87" s="74"/>
+      <c r="V87" s="74"/>
+      <c r="W87" s="74"/>
+      <c r="X87" s="74"/>
+      <c r="Y87" s="74"/>
+      <c r="Z87" s="74"/>
+      <c r="AA87" s="74"/>
+      <c r="AB87" s="74"/>
+      <c r="AC87" s="74"/>
+      <c r="AD87" s="74"/>
+      <c r="AE87" s="74"/>
+      <c r="AF87" s="74"/>
+      <c r="AG87" s="74"/>
+      <c r="AH87" s="74"/>
+      <c r="AI87" s="74"/>
+      <c r="AJ87" s="74"/>
+      <c r="AK87" s="74"/>
     </row>
     <row r="88" spans="1:37" ht="15" customHeight="1">
       <c r="B88" s="30" t="s">
@@ -13704,17 +13695,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AK132"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C74" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView topLeftCell="B1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="58" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" style="58" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" style="58" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="45.6640625" style="58" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1">
@@ -24207,44 +24193,44 @@
     </row>
     <row r="117" spans="1:37" ht="15" customHeight="1" thickBot="1"/>
     <row r="118" spans="1:37" ht="15" customHeight="1">
-      <c r="B118" s="72" t="s">
+      <c r="B118" s="73" t="s">
         <v>346</v>
       </c>
-      <c r="C118" s="73"/>
-      <c r="D118" s="73"/>
-      <c r="E118" s="73"/>
-      <c r="F118" s="73"/>
-      <c r="G118" s="73"/>
-      <c r="H118" s="73"/>
-      <c r="I118" s="73"/>
-      <c r="J118" s="73"/>
-      <c r="K118" s="73"/>
-      <c r="L118" s="73"/>
-      <c r="M118" s="73"/>
-      <c r="N118" s="73"/>
-      <c r="O118" s="73"/>
-      <c r="P118" s="73"/>
-      <c r="Q118" s="73"/>
-      <c r="R118" s="73"/>
-      <c r="S118" s="73"/>
-      <c r="T118" s="73"/>
-      <c r="U118" s="73"/>
-      <c r="V118" s="73"/>
-      <c r="W118" s="73"/>
-      <c r="X118" s="73"/>
-      <c r="Y118" s="73"/>
-      <c r="Z118" s="73"/>
-      <c r="AA118" s="73"/>
-      <c r="AB118" s="73"/>
-      <c r="AC118" s="73"/>
-      <c r="AD118" s="73"/>
-      <c r="AE118" s="73"/>
-      <c r="AF118" s="73"/>
-      <c r="AG118" s="73"/>
-      <c r="AH118" s="73"/>
-      <c r="AI118" s="73"/>
-      <c r="AJ118" s="73"/>
-      <c r="AK118" s="73"/>
+      <c r="C118" s="74"/>
+      <c r="D118" s="74"/>
+      <c r="E118" s="74"/>
+      <c r="F118" s="74"/>
+      <c r="G118" s="74"/>
+      <c r="H118" s="74"/>
+      <c r="I118" s="74"/>
+      <c r="J118" s="74"/>
+      <c r="K118" s="74"/>
+      <c r="L118" s="74"/>
+      <c r="M118" s="74"/>
+      <c r="N118" s="74"/>
+      <c r="O118" s="74"/>
+      <c r="P118" s="74"/>
+      <c r="Q118" s="74"/>
+      <c r="R118" s="74"/>
+      <c r="S118" s="74"/>
+      <c r="T118" s="74"/>
+      <c r="U118" s="74"/>
+      <c r="V118" s="74"/>
+      <c r="W118" s="74"/>
+      <c r="X118" s="74"/>
+      <c r="Y118" s="74"/>
+      <c r="Z118" s="74"/>
+      <c r="AA118" s="74"/>
+      <c r="AB118" s="74"/>
+      <c r="AC118" s="74"/>
+      <c r="AD118" s="74"/>
+      <c r="AE118" s="74"/>
+      <c r="AF118" s="74"/>
+      <c r="AG118" s="74"/>
+      <c r="AH118" s="74"/>
+      <c r="AI118" s="74"/>
+      <c r="AJ118" s="74"/>
+      <c r="AK118" s="74"/>
     </row>
     <row r="119" spans="1:37" ht="15" customHeight="1">
       <c r="B119" s="30" t="s">
@@ -24329,17 +24315,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AK76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView topLeftCell="B1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="58" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" style="58" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" style="58" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="45.6640625" style="58" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1">
@@ -29099,44 +29080,44 @@
     </row>
     <row r="66" spans="1:37" ht="15" customHeight="1" thickBot="1"/>
     <row r="67" spans="1:37" ht="15" customHeight="1">
-      <c r="B67" s="72" t="s">
+      <c r="B67" s="73" t="s">
         <v>432</v>
       </c>
-      <c r="C67" s="73"/>
-      <c r="D67" s="73"/>
-      <c r="E67" s="73"/>
-      <c r="F67" s="73"/>
-      <c r="G67" s="73"/>
-      <c r="H67" s="73"/>
-      <c r="I67" s="73"/>
-      <c r="J67" s="73"/>
-      <c r="K67" s="73"/>
-      <c r="L67" s="73"/>
-      <c r="M67" s="73"/>
-      <c r="N67" s="73"/>
-      <c r="O67" s="73"/>
-      <c r="P67" s="73"/>
-      <c r="Q67" s="73"/>
-      <c r="R67" s="73"/>
-      <c r="S67" s="73"/>
-      <c r="T67" s="73"/>
-      <c r="U67" s="73"/>
-      <c r="V67" s="73"/>
-      <c r="W67" s="73"/>
-      <c r="X67" s="73"/>
-      <c r="Y67" s="73"/>
-      <c r="Z67" s="73"/>
-      <c r="AA67" s="73"/>
-      <c r="AB67" s="73"/>
-      <c r="AC67" s="73"/>
-      <c r="AD67" s="73"/>
-      <c r="AE67" s="73"/>
-      <c r="AF67" s="73"/>
-      <c r="AG67" s="73"/>
-      <c r="AH67" s="73"/>
-      <c r="AI67" s="73"/>
-      <c r="AJ67" s="73"/>
-      <c r="AK67" s="73"/>
+      <c r="C67" s="74"/>
+      <c r="D67" s="74"/>
+      <c r="E67" s="74"/>
+      <c r="F67" s="74"/>
+      <c r="G67" s="74"/>
+      <c r="H67" s="74"/>
+      <c r="I67" s="74"/>
+      <c r="J67" s="74"/>
+      <c r="K67" s="74"/>
+      <c r="L67" s="74"/>
+      <c r="M67" s="74"/>
+      <c r="N67" s="74"/>
+      <c r="O67" s="74"/>
+      <c r="P67" s="74"/>
+      <c r="Q67" s="74"/>
+      <c r="R67" s="74"/>
+      <c r="S67" s="74"/>
+      <c r="T67" s="74"/>
+      <c r="U67" s="74"/>
+      <c r="V67" s="74"/>
+      <c r="W67" s="74"/>
+      <c r="X67" s="74"/>
+      <c r="Y67" s="74"/>
+      <c r="Z67" s="74"/>
+      <c r="AA67" s="74"/>
+      <c r="AB67" s="74"/>
+      <c r="AC67" s="74"/>
+      <c r="AD67" s="74"/>
+      <c r="AE67" s="74"/>
+      <c r="AF67" s="74"/>
+      <c r="AG67" s="74"/>
+      <c r="AH67" s="74"/>
+      <c r="AI67" s="74"/>
+      <c r="AJ67" s="74"/>
+      <c r="AK67" s="74"/>
     </row>
     <row r="68" spans="1:37" ht="15" customHeight="1">
       <c r="B68" s="30" t="s">
@@ -29198,12 +29179,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" style="58" customWidth="1"/>
+    <col min="1" max="1" width="34.6640625" style="58" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="15.95" customHeight="1" thickBot="1">
+    <row r="1" spans="1:36" ht="16" customHeight="1" thickBot="1">
       <c r="A1" s="9" t="s">
         <v>62</v>
       </c>
@@ -29310,7 +29291,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="15.95" customHeight="1" thickTop="1"/>
+    <row r="2" spans="1:36" ht="16" customHeight="1" thickTop="1"/>
     <row r="3" spans="1:36">
       <c r="B3" s="28" t="s">
         <v>63</v>
@@ -29357,7 +29338,7 @@
       <c r="E6" s="28"/>
       <c r="F6" s="28"/>
     </row>
-    <row r="10" spans="1:36" ht="15.95" customHeight="1">
+    <row r="10" spans="1:36" ht="16" customHeight="1">
       <c r="A10" s="10" t="s">
         <v>441</v>
       </c>
@@ -29407,7 +29388,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:36" ht="15.95" customHeight="1" thickBot="1">
+    <row r="13" spans="1:36" ht="16" customHeight="1" thickBot="1">
       <c r="A13" s="8" t="s">
         <v>363</v>
       </c>
@@ -29517,7 +29498,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="14" spans="1:36" ht="15.95" customHeight="1" thickTop="1"/>
+    <row r="14" spans="1:36" ht="16" customHeight="1" thickTop="1"/>
     <row r="15" spans="1:36">
       <c r="A15" s="4" t="s">
         <v>364</v>
@@ -29528,7 +29509,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="17" spans="1:36" ht="15.95" customHeight="1">
+    <row r="17" spans="1:36" ht="16" customHeight="1">
       <c r="A17" s="7" t="s">
         <v>367</v>
       </c>
@@ -29638,7 +29619,7 @@
         <v>-1.0081E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:36" ht="15.95" customHeight="1">
+    <row r="18" spans="1:36" ht="16" customHeight="1">
       <c r="A18" s="7" t="s">
         <v>369</v>
       </c>
@@ -29748,7 +29729,7 @@
         <v>3.0148999999999999E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:36" ht="15.95" customHeight="1">
+    <row r="19" spans="1:36" ht="16" customHeight="1">
       <c r="A19" s="7" t="s">
         <v>371</v>
       </c>
@@ -29863,7 +29844,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="22" spans="1:36" ht="15.95" customHeight="1">
+    <row r="22" spans="1:36" ht="16" customHeight="1">
       <c r="A22" s="7" t="s">
         <v>374</v>
       </c>
@@ -29973,7 +29954,7 @@
         <v>-1.7652999999999999E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:36" ht="15.95" customHeight="1">
+    <row r="23" spans="1:36" ht="16" customHeight="1">
       <c r="A23" s="7" t="s">
         <v>376</v>
       </c>
@@ -30083,7 +30064,7 @@
         <v>7.2267999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:36" ht="15.95" customHeight="1">
+    <row r="24" spans="1:36" ht="16" customHeight="1">
       <c r="A24" s="7" t="s">
         <v>378</v>
       </c>
@@ -30193,7 +30174,7 @@
         <v>7.4912999999999993E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:36" ht="15.95" customHeight="1">
+    <row r="25" spans="1:36" ht="16" customHeight="1">
       <c r="A25" s="7" t="s">
         <v>380</v>
       </c>
@@ -30303,7 +30284,7 @@
         <v>0.12363499999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:36" ht="15.95" customHeight="1">
+    <row r="26" spans="1:36" ht="16" customHeight="1">
       <c r="A26" s="7" t="s">
         <v>382</v>
       </c>
@@ -30413,7 +30394,7 @@
         <v>5.9776000000000003E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:36" ht="15.95" customHeight="1">
+    <row r="27" spans="1:36" ht="16" customHeight="1">
       <c r="A27" s="7" t="s">
         <v>384</v>
       </c>
@@ -30523,7 +30504,7 @@
         <v>6.5015000000000003E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:36" ht="15.95" customHeight="1">
+    <row r="28" spans="1:36" ht="16" customHeight="1">
       <c r="A28" s="7" t="s">
         <v>386</v>
       </c>
@@ -30633,7 +30614,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="29" spans="1:36" ht="15.95" customHeight="1">
+    <row r="29" spans="1:36" ht="16" customHeight="1">
       <c r="A29" s="7" t="s">
         <v>388</v>
       </c>
@@ -30743,7 +30724,7 @@
         <v>2.4118000000000001E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:36" ht="15.95" customHeight="1">
+    <row r="30" spans="1:36" ht="16" customHeight="1">
       <c r="A30" s="7" t="s">
         <v>390</v>
       </c>
@@ -30853,7 +30834,7 @@
         <v>-3.8976999999999998E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:36" ht="15.95" customHeight="1">
+    <row r="31" spans="1:36" ht="16" customHeight="1">
       <c r="A31" s="7" t="s">
         <v>392</v>
       </c>
@@ -30963,7 +30944,7 @@
         <v>-4.5399999999999998E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:36" ht="15.95" customHeight="1">
+    <row r="32" spans="1:36" ht="16" customHeight="1">
       <c r="A32" s="7" t="s">
         <v>394</v>
       </c>
@@ -31073,7 +31054,7 @@
         <v>6.0499999999999998E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:36" ht="15.95" customHeight="1">
+    <row r="33" spans="1:36" ht="16" customHeight="1">
       <c r="A33" s="7" t="s">
         <v>396</v>
       </c>
@@ -31183,7 +31164,7 @@
         <v>7.4590000000000004E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:36" ht="15.95" customHeight="1">
+    <row r="34" spans="1:36" ht="16" customHeight="1">
       <c r="A34" s="7" t="s">
         <v>398</v>
       </c>
@@ -31293,7 +31274,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="35" spans="1:36" ht="15.95" customHeight="1">
+    <row r="35" spans="1:36" ht="16" customHeight="1">
       <c r="A35" s="7" t="s">
         <v>400</v>
       </c>
@@ -31403,7 +31384,7 @@
         <v>0.10102700000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:36" ht="15.95" customHeight="1">
+    <row r="36" spans="1:36" ht="16" customHeight="1">
       <c r="A36" s="7" t="s">
         <v>402</v>
       </c>
@@ -31513,7 +31494,7 @@
         <v>2.5113E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:36" ht="15.95" customHeight="1">
+    <row r="38" spans="1:36" ht="16" customHeight="1">
       <c r="A38" s="7" t="s">
         <v>443</v>
       </c>
@@ -31633,7 +31614,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="42" spans="1:36" ht="15.95" customHeight="1">
+    <row r="42" spans="1:36" ht="16" customHeight="1">
       <c r="A42" s="7" t="s">
         <v>367</v>
       </c>
@@ -31743,7 +31724,7 @@
         <v>-2.3338000000000001E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:36" ht="15.95" customHeight="1">
+    <row r="43" spans="1:36" ht="16" customHeight="1">
       <c r="A43" s="7" t="s">
         <v>369</v>
       </c>
@@ -31853,7 +31834,7 @@
         <v>3.2419000000000003E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:36" ht="15.95" customHeight="1">
+    <row r="44" spans="1:36" ht="16" customHeight="1">
       <c r="A44" s="7" t="s">
         <v>410</v>
       </c>
@@ -31968,7 +31949,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="47" spans="1:36" ht="15.95" customHeight="1">
+    <row r="47" spans="1:36" ht="16" customHeight="1">
       <c r="A47" s="7" t="s">
         <v>374</v>
       </c>
@@ -32078,7 +32059,7 @@
         <v>-2.4993999999999999E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:36" ht="15.95" customHeight="1">
+    <row r="48" spans="1:36" ht="16" customHeight="1">
       <c r="A48" s="7" t="s">
         <v>376</v>
       </c>
@@ -32188,7 +32169,7 @@
         <v>0.100457</v>
       </c>
     </row>
-    <row r="49" spans="1:36" ht="15.95" customHeight="1">
+    <row r="49" spans="1:36" ht="16" customHeight="1">
       <c r="A49" s="7" t="s">
         <v>378</v>
       </c>
@@ -32298,7 +32279,7 @@
         <v>0.11165899999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:36" ht="15.95" customHeight="1">
+    <row r="50" spans="1:36" ht="16" customHeight="1">
       <c r="A50" s="7" t="s">
         <v>380</v>
       </c>
@@ -32408,7 +32389,7 @@
         <v>0.118467</v>
       </c>
     </row>
-    <row r="51" spans="1:36" ht="15.95" customHeight="1">
+    <row r="51" spans="1:36" ht="16" customHeight="1">
       <c r="A51" s="7" t="s">
         <v>382</v>
       </c>
@@ -32518,7 +32499,7 @@
         <v>6.7011000000000001E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:36" ht="15.95" customHeight="1">
+    <row r="52" spans="1:36" ht="16" customHeight="1">
       <c r="A52" s="7" t="s">
         <v>384</v>
       </c>
@@ -32628,7 +32609,7 @@
         <v>7.2749999999999995E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:36" ht="15.95" customHeight="1">
+    <row r="53" spans="1:36" ht="16" customHeight="1">
       <c r="A53" s="7" t="s">
         <v>386</v>
       </c>
@@ -32738,7 +32719,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="54" spans="1:36" ht="15.95" customHeight="1">
+    <row r="54" spans="1:36" ht="16" customHeight="1">
       <c r="A54" s="7" t="s">
         <v>388</v>
       </c>
@@ -32848,7 +32829,7 @@
         <v>3.6835E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:36" ht="15.95" customHeight="1">
+    <row r="55" spans="1:36" ht="16" customHeight="1">
       <c r="A55" s="7" t="s">
         <v>390</v>
       </c>
@@ -32958,7 +32939,7 @@
         <v>-3.9047999999999999E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:36" ht="15.95" customHeight="1">
+    <row r="56" spans="1:36" ht="16" customHeight="1">
       <c r="A56" s="7" t="s">
         <v>392</v>
       </c>
@@ -33068,7 +33049,7 @@
         <v>-9.3220000000000004E-3</v>
       </c>
     </row>
-    <row r="57" spans="1:36" ht="15.95" customHeight="1">
+    <row r="57" spans="1:36" ht="16" customHeight="1">
       <c r="A57" s="7" t="s">
         <v>394</v>
       </c>
@@ -33178,7 +33159,7 @@
         <v>-3.1987000000000002E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:36" ht="15.95" customHeight="1">
+    <row r="58" spans="1:36" ht="16" customHeight="1">
       <c r="A58" s="7" t="s">
         <v>396</v>
       </c>
@@ -33288,7 +33269,7 @@
         <v>-4.3679999999999997E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:36" ht="15.95" customHeight="1">
+    <row r="59" spans="1:36" ht="16" customHeight="1">
       <c r="A59" s="7" t="s">
         <v>398</v>
       </c>
@@ -33398,7 +33379,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="60" spans="1:36" ht="15.95" customHeight="1">
+    <row r="60" spans="1:36" ht="16" customHeight="1">
       <c r="A60" s="7" t="s">
         <v>400</v>
       </c>
@@ -33508,7 +33489,7 @@
         <v>9.9144999999999997E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:36" ht="15.95" customHeight="1">
+    <row r="61" spans="1:36" ht="16" customHeight="1">
       <c r="A61" s="7" t="s">
         <v>427</v>
       </c>
@@ -33618,7 +33599,7 @@
         <v>-1.088E-3</v>
       </c>
     </row>
-    <row r="63" spans="1:36" ht="15.95" customHeight="1">
+    <row r="63" spans="1:36" ht="16" customHeight="1">
       <c r="A63" s="7" t="s">
         <v>444</v>
       </c>
@@ -33843,7 +33824,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="68" spans="1:36" ht="15.95" customHeight="1">
+    <row r="68" spans="1:36" ht="16" customHeight="1">
       <c r="A68" s="7" t="s">
         <v>447</v>
       </c>
@@ -33953,7 +33934,7 @@
         <v>-2.1242E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:36" ht="15.95" customHeight="1">
+    <row r="69" spans="1:36" ht="16" customHeight="1">
       <c r="A69" s="7" t="s">
         <v>448</v>
       </c>
@@ -34063,7 +34044,7 @@
         <v>9.3869999999999995E-3</v>
       </c>
     </row>
-    <row r="70" spans="1:36" ht="15.95" customHeight="1">
+    <row r="70" spans="1:36" ht="16" customHeight="1">
       <c r="A70" s="7" t="s">
         <v>449</v>
       </c>
@@ -34173,7 +34154,7 @@
         <v>0.12775</v>
       </c>
     </row>
-    <row r="71" spans="1:36" ht="15.95" customHeight="1">
+    <row r="71" spans="1:36" ht="16" customHeight="1">
       <c r="A71" s="7" t="s">
         <v>450</v>
       </c>
@@ -34283,7 +34264,7 @@
         <v>2.8726000000000002E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:36" ht="15.95" customHeight="1">
+    <row r="72" spans="1:36" ht="16" customHeight="1">
       <c r="A72" s="7" t="s">
         <v>451</v>
       </c>
@@ -34393,7 +34374,7 @@
         <v>5.5759999999999997E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:36" ht="15.95" customHeight="1">
+    <row r="73" spans="1:36" ht="16" customHeight="1">
       <c r="A73" s="7" t="s">
         <v>452</v>
       </c>
@@ -34503,7 +34484,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="74" spans="1:36" ht="15.95" customHeight="1">
+    <row r="74" spans="1:36" ht="16" customHeight="1">
       <c r="A74" s="7" t="s">
         <v>453</v>
       </c>
@@ -34613,7 +34594,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="75" spans="1:36" ht="15.95" customHeight="1">
+    <row r="75" spans="1:36" ht="16" customHeight="1">
       <c r="A75" s="7" t="s">
         <v>454</v>
       </c>
@@ -34723,7 +34704,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="76" spans="1:36" ht="15.95" customHeight="1">
+    <row r="76" spans="1:36" ht="16" customHeight="1">
       <c r="A76" s="7" t="s">
         <v>455</v>
       </c>
@@ -34943,46 +34924,46 @@
         <v>1.0678999999999999E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:36" ht="15.95" customHeight="1" thickBot="1"/>
+    <row r="78" spans="1:36" ht="16" customHeight="1" thickBot="1"/>
     <row r="79" spans="1:36">
-      <c r="A79" s="72" t="s">
+      <c r="A79" s="73" t="s">
         <v>457</v>
       </c>
-      <c r="B79" s="73"/>
-      <c r="C79" s="73"/>
-      <c r="D79" s="73"/>
-      <c r="E79" s="73"/>
-      <c r="F79" s="73"/>
-      <c r="G79" s="73"/>
-      <c r="H79" s="73"/>
-      <c r="I79" s="73"/>
-      <c r="J79" s="73"/>
-      <c r="K79" s="73"/>
-      <c r="L79" s="73"/>
-      <c r="M79" s="73"/>
-      <c r="N79" s="73"/>
-      <c r="O79" s="73"/>
-      <c r="P79" s="73"/>
-      <c r="Q79" s="73"/>
-      <c r="R79" s="73"/>
-      <c r="S79" s="73"/>
-      <c r="T79" s="73"/>
-      <c r="U79" s="73"/>
-      <c r="V79" s="73"/>
-      <c r="W79" s="73"/>
-      <c r="X79" s="73"/>
-      <c r="Y79" s="73"/>
-      <c r="Z79" s="73"/>
-      <c r="AA79" s="73"/>
-      <c r="AB79" s="73"/>
-      <c r="AC79" s="73"/>
-      <c r="AD79" s="73"/>
-      <c r="AE79" s="73"/>
-      <c r="AF79" s="73"/>
-      <c r="AG79" s="73"/>
-      <c r="AH79" s="73"/>
-      <c r="AI79" s="73"/>
-      <c r="AJ79" s="73"/>
+      <c r="B79" s="74"/>
+      <c r="C79" s="74"/>
+      <c r="D79" s="74"/>
+      <c r="E79" s="74"/>
+      <c r="F79" s="74"/>
+      <c r="G79" s="74"/>
+      <c r="H79" s="74"/>
+      <c r="I79" s="74"/>
+      <c r="J79" s="74"/>
+      <c r="K79" s="74"/>
+      <c r="L79" s="74"/>
+      <c r="M79" s="74"/>
+      <c r="N79" s="74"/>
+      <c r="O79" s="74"/>
+      <c r="P79" s="74"/>
+      <c r="Q79" s="74"/>
+      <c r="R79" s="74"/>
+      <c r="S79" s="74"/>
+      <c r="T79" s="74"/>
+      <c r="U79" s="74"/>
+      <c r="V79" s="74"/>
+      <c r="W79" s="74"/>
+      <c r="X79" s="74"/>
+      <c r="Y79" s="74"/>
+      <c r="Z79" s="74"/>
+      <c r="AA79" s="74"/>
+      <c r="AB79" s="74"/>
+      <c r="AC79" s="74"/>
+      <c r="AD79" s="74"/>
+      <c r="AE79" s="74"/>
+      <c r="AF79" s="74"/>
+      <c r="AG79" s="74"/>
+      <c r="AH79" s="74"/>
+      <c r="AI79" s="74"/>
+      <c r="AJ79" s="74"/>
     </row>
     <row r="80" spans="1:36">
       <c r="A80" s="30" t="s">
@@ -35036,17 +35017,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AK198"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView topLeftCell="B1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="58" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" style="58" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" style="58" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="45.6640625" style="58" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1">
@@ -54935,44 +54911,44 @@
       </c>
     </row>
     <row r="198" spans="1:37" ht="15" customHeight="1">
-      <c r="B198" s="72" t="s">
+      <c r="B198" s="73" t="s">
         <v>659</v>
       </c>
-      <c r="C198" s="73"/>
-      <c r="D198" s="73"/>
-      <c r="E198" s="73"/>
-      <c r="F198" s="73"/>
-      <c r="G198" s="73"/>
-      <c r="H198" s="73"/>
-      <c r="I198" s="73"/>
-      <c r="J198" s="73"/>
-      <c r="K198" s="73"/>
-      <c r="L198" s="73"/>
-      <c r="M198" s="73"/>
-      <c r="N198" s="73"/>
-      <c r="O198" s="73"/>
-      <c r="P198" s="73"/>
-      <c r="Q198" s="73"/>
-      <c r="R198" s="73"/>
-      <c r="S198" s="73"/>
-      <c r="T198" s="73"/>
-      <c r="U198" s="73"/>
-      <c r="V198" s="73"/>
-      <c r="W198" s="73"/>
-      <c r="X198" s="73"/>
-      <c r="Y198" s="73"/>
-      <c r="Z198" s="73"/>
-      <c r="AA198" s="73"/>
-      <c r="AB198" s="73"/>
-      <c r="AC198" s="73"/>
-      <c r="AD198" s="73"/>
-      <c r="AE198" s="73"/>
-      <c r="AF198" s="73"/>
-      <c r="AG198" s="73"/>
-      <c r="AH198" s="73"/>
-      <c r="AI198" s="73"/>
-      <c r="AJ198" s="73"/>
-      <c r="AK198" s="73"/>
+      <c r="C198" s="74"/>
+      <c r="D198" s="74"/>
+      <c r="E198" s="74"/>
+      <c r="F198" s="74"/>
+      <c r="G198" s="74"/>
+      <c r="H198" s="74"/>
+      <c r="I198" s="74"/>
+      <c r="J198" s="74"/>
+      <c r="K198" s="74"/>
+      <c r="L198" s="74"/>
+      <c r="M198" s="74"/>
+      <c r="N198" s="74"/>
+      <c r="O198" s="74"/>
+      <c r="P198" s="74"/>
+      <c r="Q198" s="74"/>
+      <c r="R198" s="74"/>
+      <c r="S198" s="74"/>
+      <c r="T198" s="74"/>
+      <c r="U198" s="74"/>
+      <c r="V198" s="74"/>
+      <c r="W198" s="74"/>
+      <c r="X198" s="74"/>
+      <c r="Y198" s="74"/>
+      <c r="Z198" s="74"/>
+      <c r="AA198" s="74"/>
+      <c r="AB198" s="74"/>
+      <c r="AC198" s="74"/>
+      <c r="AD198" s="74"/>
+      <c r="AE198" s="74"/>
+      <c r="AF198" s="74"/>
+      <c r="AG198" s="74"/>
+      <c r="AH198" s="74"/>
+      <c r="AI198" s="74"/>
+      <c r="AJ198" s="74"/>
+      <c r="AK198" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -54987,17 +54963,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AK286"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView topLeftCell="B1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="58" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" style="58" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" style="58" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="45.6640625" style="58" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="15" customHeight="1" thickBot="1">
@@ -79665,44 +79636,44 @@
     </row>
     <row r="274" spans="1:37" ht="15" customHeight="1" thickBot="1"/>
     <row r="275" spans="1:37" ht="15" customHeight="1">
-      <c r="B275" s="72" t="s">
+      <c r="B275" s="73" t="s">
         <v>920</v>
       </c>
-      <c r="C275" s="73"/>
-      <c r="D275" s="73"/>
-      <c r="E275" s="73"/>
-      <c r="F275" s="73"/>
-      <c r="G275" s="73"/>
-      <c r="H275" s="73"/>
-      <c r="I275" s="73"/>
-      <c r="J275" s="73"/>
-      <c r="K275" s="73"/>
-      <c r="L275" s="73"/>
-      <c r="M275" s="73"/>
-      <c r="N275" s="73"/>
-      <c r="O275" s="73"/>
-      <c r="P275" s="73"/>
-      <c r="Q275" s="73"/>
-      <c r="R275" s="73"/>
-      <c r="S275" s="73"/>
-      <c r="T275" s="73"/>
-      <c r="U275" s="73"/>
-      <c r="V275" s="73"/>
-      <c r="W275" s="73"/>
-      <c r="X275" s="73"/>
-      <c r="Y275" s="73"/>
-      <c r="Z275" s="73"/>
-      <c r="AA275" s="73"/>
-      <c r="AB275" s="73"/>
-      <c r="AC275" s="73"/>
-      <c r="AD275" s="73"/>
-      <c r="AE275" s="73"/>
-      <c r="AF275" s="73"/>
-      <c r="AG275" s="73"/>
-      <c r="AH275" s="73"/>
-      <c r="AI275" s="73"/>
-      <c r="AJ275" s="73"/>
-      <c r="AK275" s="73"/>
+      <c r="C275" s="74"/>
+      <c r="D275" s="74"/>
+      <c r="E275" s="74"/>
+      <c r="F275" s="74"/>
+      <c r="G275" s="74"/>
+      <c r="H275" s="74"/>
+      <c r="I275" s="74"/>
+      <c r="J275" s="74"/>
+      <c r="K275" s="74"/>
+      <c r="L275" s="74"/>
+      <c r="M275" s="74"/>
+      <c r="N275" s="74"/>
+      <c r="O275" s="74"/>
+      <c r="P275" s="74"/>
+      <c r="Q275" s="74"/>
+      <c r="R275" s="74"/>
+      <c r="S275" s="74"/>
+      <c r="T275" s="74"/>
+      <c r="U275" s="74"/>
+      <c r="V275" s="74"/>
+      <c r="W275" s="74"/>
+      <c r="X275" s="74"/>
+      <c r="Y275" s="74"/>
+      <c r="Z275" s="74"/>
+      <c r="AA275" s="74"/>
+      <c r="AB275" s="74"/>
+      <c r="AC275" s="74"/>
+      <c r="AD275" s="74"/>
+      <c r="AE275" s="74"/>
+      <c r="AF275" s="74"/>
+      <c r="AG275" s="74"/>
+      <c r="AH275" s="74"/>
+      <c r="AI275" s="74"/>
+      <c r="AJ275" s="74"/>
+      <c r="AK275" s="74"/>
     </row>
     <row r="276" spans="1:37" ht="15" customHeight="1">
       <c r="B276" s="30" t="s">
@@ -79776,59 +79747,59 @@
   <dimension ref="A1:AK121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AK31" sqref="AK31"/>
+      <selection sqref="A1:AI1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="35" style="38" customWidth="1"/>
-    <col min="2" max="3" width="9.85546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="4" max="19" width="10.85546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.85546875" style="27" bestFit="1" customWidth="1"/>
-    <col min="21" max="34" width="10.85546875" style="38" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="9.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="36" max="39" width="9.140625" style="38" customWidth="1"/>
-    <col min="40" max="16384" width="9.140625" style="38"/>
+    <col min="2" max="3" width="9.83203125" style="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="19" width="10.83203125" style="38" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.83203125" style="27" bestFit="1" customWidth="1"/>
+    <col min="21" max="34" width="10.83203125" style="38" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="9.33203125" style="38" bestFit="1" customWidth="1"/>
+    <col min="36" max="42" width="9.1640625" style="38" customWidth="1"/>
+    <col min="43" max="16384" width="9.1640625" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="16.5" customHeight="1" thickBot="1">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="92" t="s">
         <v>928</v>
       </c>
-      <c r="B1" s="85"/>
-      <c r="C1" s="85"/>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-      <c r="F1" s="85"/>
-      <c r="G1" s="85"/>
-      <c r="H1" s="85"/>
-      <c r="I1" s="85"/>
-      <c r="J1" s="85"/>
-      <c r="K1" s="85"/>
-      <c r="L1" s="85"/>
-      <c r="M1" s="85"/>
-      <c r="N1" s="85"/>
-      <c r="O1" s="85"/>
-      <c r="P1" s="85"/>
-      <c r="Q1" s="85"/>
-      <c r="R1" s="85"/>
-      <c r="S1" s="85"/>
-      <c r="T1" s="85"/>
-      <c r="U1" s="85"/>
-      <c r="V1" s="85"/>
-      <c r="W1" s="85"/>
-      <c r="X1" s="85"/>
-      <c r="Y1" s="85"/>
-      <c r="Z1" s="85"/>
-      <c r="AA1" s="85"/>
-      <c r="AB1" s="85"/>
-      <c r="AC1" s="85"/>
-      <c r="AD1" s="85"/>
-      <c r="AE1" s="85"/>
-      <c r="AF1" s="85"/>
-      <c r="AG1" s="85"/>
-      <c r="AH1" s="85"/>
-      <c r="AI1" s="85"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="93"/>
+      <c r="L1" s="93"/>
+      <c r="M1" s="93"/>
+      <c r="N1" s="93"/>
+      <c r="O1" s="93"/>
+      <c r="P1" s="93"/>
+      <c r="Q1" s="93"/>
+      <c r="R1" s="93"/>
+      <c r="S1" s="93"/>
+      <c r="T1" s="93"/>
+      <c r="U1" s="93"/>
+      <c r="V1" s="93"/>
+      <c r="W1" s="93"/>
+      <c r="X1" s="93"/>
+      <c r="Y1" s="93"/>
+      <c r="Z1" s="93"/>
+      <c r="AA1" s="93"/>
+      <c r="AB1" s="93"/>
+      <c r="AC1" s="93"/>
+      <c r="AD1" s="93"/>
+      <c r="AE1" s="93"/>
+      <c r="AF1" s="93"/>
+      <c r="AG1" s="93"/>
+      <c r="AH1" s="93"/>
+      <c r="AI1" s="93"/>
     </row>
     <row r="2" spans="1:37" s="19" customFormat="1" ht="16.5" customHeight="1">
       <c r="A2" s="31"/>
@@ -83091,27 +83062,27 @@
         <v>11961568</v>
       </c>
     </row>
-    <row r="35" spans="1:35" s="70" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A35" s="86" t="s">
+    <row r="35" spans="1:35" s="72" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A35" s="94" t="s">
         <v>963</v>
       </c>
-      <c r="B35" s="87"/>
-      <c r="C35" s="87"/>
-      <c r="D35" s="87"/>
-      <c r="E35" s="87"/>
-      <c r="F35" s="87"/>
-      <c r="G35" s="87"/>
-      <c r="H35" s="87"/>
-      <c r="I35" s="87"/>
-      <c r="J35" s="87"/>
-      <c r="K35" s="87"/>
-      <c r="L35" s="87"/>
-      <c r="M35" s="87"/>
-      <c r="N35" s="87"/>
-      <c r="O35" s="87"/>
-      <c r="P35" s="87"/>
-      <c r="Q35" s="87"/>
-      <c r="R35" s="87"/>
+      <c r="B35" s="95"/>
+      <c r="C35" s="95"/>
+      <c r="D35" s="95"/>
+      <c r="E35" s="95"/>
+      <c r="F35" s="95"/>
+      <c r="G35" s="95"/>
+      <c r="H35" s="95"/>
+      <c r="I35" s="95"/>
+      <c r="J35" s="95"/>
+      <c r="K35" s="95"/>
+      <c r="L35" s="95"/>
+      <c r="M35" s="95"/>
+      <c r="N35" s="95"/>
+      <c r="O35" s="95"/>
+      <c r="P35" s="95"/>
+      <c r="Q35" s="95"/>
+      <c r="R35" s="95"/>
       <c r="S35" s="54"/>
       <c r="T35" s="54"/>
       <c r="U35" s="54"/>
@@ -83125,1250 +83096,1250 @@
       <c r="AC35" s="54"/>
       <c r="AE35" s="55"/>
     </row>
-    <row r="36" spans="1:35" s="70" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A36" s="88"/>
-      <c r="B36" s="89"/>
-      <c r="C36" s="89"/>
-      <c r="D36" s="89"/>
-      <c r="E36" s="89"/>
-      <c r="F36" s="89"/>
-      <c r="G36" s="89"/>
-      <c r="H36" s="89"/>
-      <c r="I36" s="89"/>
-      <c r="J36" s="89"/>
-      <c r="K36" s="89"/>
-      <c r="L36" s="89"/>
-      <c r="M36" s="89"/>
-      <c r="N36" s="89"/>
-      <c r="O36" s="89"/>
-      <c r="P36" s="89"/>
-      <c r="Q36" s="89"/>
-      <c r="R36" s="89"/>
-    </row>
-    <row r="37" spans="1:35" s="68" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A37" s="90" t="s">
+    <row r="36" spans="1:35" s="72" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A36" s="89"/>
+      <c r="B36" s="96"/>
+      <c r="C36" s="96"/>
+      <c r="D36" s="96"/>
+      <c r="E36" s="96"/>
+      <c r="F36" s="96"/>
+      <c r="G36" s="96"/>
+      <c r="H36" s="96"/>
+      <c r="I36" s="96"/>
+      <c r="J36" s="96"/>
+      <c r="K36" s="96"/>
+      <c r="L36" s="96"/>
+      <c r="M36" s="96"/>
+      <c r="N36" s="96"/>
+      <c r="O36" s="96"/>
+      <c r="P36" s="96"/>
+      <c r="Q36" s="96"/>
+      <c r="R36" s="96"/>
+    </row>
+    <row r="37" spans="1:35" s="70" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A37" s="97" t="s">
         <v>964</v>
       </c>
-      <c r="B37" s="75"/>
-      <c r="C37" s="75"/>
-      <c r="D37" s="75"/>
-      <c r="E37" s="75"/>
-      <c r="F37" s="75"/>
-      <c r="G37" s="75"/>
-      <c r="H37" s="75"/>
-      <c r="I37" s="75"/>
-      <c r="J37" s="75"/>
-      <c r="K37" s="75"/>
-      <c r="L37" s="75"/>
-      <c r="M37" s="75"/>
-      <c r="N37" s="75"/>
-      <c r="O37" s="75"/>
-      <c r="P37" s="75"/>
-      <c r="Q37" s="75"/>
-      <c r="R37" s="75"/>
-    </row>
-    <row r="38" spans="1:35" s="68" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A38" s="83" t="s">
+      <c r="B37" s="76"/>
+      <c r="C37" s="76"/>
+      <c r="D37" s="76"/>
+      <c r="E37" s="76"/>
+      <c r="F37" s="76"/>
+      <c r="G37" s="76"/>
+      <c r="H37" s="76"/>
+      <c r="I37" s="76"/>
+      <c r="J37" s="76"/>
+      <c r="K37" s="76"/>
+      <c r="L37" s="76"/>
+      <c r="M37" s="76"/>
+      <c r="N37" s="76"/>
+      <c r="O37" s="76"/>
+      <c r="P37" s="76"/>
+      <c r="Q37" s="76"/>
+      <c r="R37" s="76"/>
+    </row>
+    <row r="38" spans="1:35" s="70" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A38" s="75" t="s">
         <v>965</v>
       </c>
-      <c r="B38" s="75"/>
-      <c r="C38" s="75"/>
-      <c r="D38" s="75"/>
-      <c r="E38" s="75"/>
-      <c r="F38" s="75"/>
-      <c r="G38" s="75"/>
-      <c r="H38" s="75"/>
-      <c r="I38" s="75"/>
-      <c r="J38" s="75"/>
-      <c r="K38" s="75"/>
-      <c r="L38" s="75"/>
-      <c r="M38" s="75"/>
-      <c r="N38" s="75"/>
-      <c r="O38" s="75"/>
-      <c r="P38" s="75"/>
-      <c r="Q38" s="75"/>
-      <c r="R38" s="75"/>
-    </row>
-    <row r="39" spans="1:35" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A39" s="74" t="s">
+      <c r="B38" s="76"/>
+      <c r="C38" s="76"/>
+      <c r="D38" s="76"/>
+      <c r="E38" s="76"/>
+      <c r="F38" s="76"/>
+      <c r="G38" s="76"/>
+      <c r="H38" s="76"/>
+      <c r="I38" s="76"/>
+      <c r="J38" s="76"/>
+      <c r="K38" s="76"/>
+      <c r="L38" s="76"/>
+      <c r="M38" s="76"/>
+      <c r="N38" s="76"/>
+      <c r="O38" s="76"/>
+      <c r="P38" s="76"/>
+      <c r="Q38" s="76"/>
+      <c r="R38" s="76"/>
+    </row>
+    <row r="39" spans="1:35" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A39" s="77" t="s">
         <v>966</v>
       </c>
-      <c r="B39" s="75"/>
-      <c r="C39" s="75"/>
-      <c r="D39" s="75"/>
-      <c r="E39" s="75"/>
-      <c r="F39" s="75"/>
-      <c r="G39" s="75"/>
-      <c r="H39" s="75"/>
-      <c r="I39" s="75"/>
-      <c r="J39" s="75"/>
-      <c r="K39" s="75"/>
-      <c r="L39" s="75"/>
-      <c r="M39" s="75"/>
-      <c r="N39" s="75"/>
-      <c r="O39" s="75"/>
-      <c r="P39" s="75"/>
-      <c r="Q39" s="75"/>
-      <c r="R39" s="75"/>
-    </row>
-    <row r="40" spans="1:35" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A40" s="83" t="s">
+      <c r="B39" s="76"/>
+      <c r="C39" s="76"/>
+      <c r="D39" s="76"/>
+      <c r="E39" s="76"/>
+      <c r="F39" s="76"/>
+      <c r="G39" s="76"/>
+      <c r="H39" s="76"/>
+      <c r="I39" s="76"/>
+      <c r="J39" s="76"/>
+      <c r="K39" s="76"/>
+      <c r="L39" s="76"/>
+      <c r="M39" s="76"/>
+      <c r="N39" s="76"/>
+      <c r="O39" s="76"/>
+      <c r="P39" s="76"/>
+      <c r="Q39" s="76"/>
+      <c r="R39" s="76"/>
+    </row>
+    <row r="40" spans="1:35" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A40" s="75" t="s">
         <v>967</v>
       </c>
-      <c r="B40" s="75"/>
-      <c r="C40" s="75"/>
-      <c r="D40" s="75"/>
-      <c r="E40" s="75"/>
-      <c r="F40" s="75"/>
-      <c r="G40" s="75"/>
-      <c r="H40" s="75"/>
-      <c r="I40" s="75"/>
-      <c r="J40" s="75"/>
-      <c r="K40" s="75"/>
-      <c r="L40" s="75"/>
-      <c r="M40" s="75"/>
-      <c r="N40" s="75"/>
-      <c r="O40" s="75"/>
-      <c r="P40" s="75"/>
-      <c r="Q40" s="75"/>
-      <c r="R40" s="75"/>
-    </row>
-    <row r="41" spans="1:35" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A41" s="83" t="s">
+      <c r="B40" s="76"/>
+      <c r="C40" s="76"/>
+      <c r="D40" s="76"/>
+      <c r="E40" s="76"/>
+      <c r="F40" s="76"/>
+      <c r="G40" s="76"/>
+      <c r="H40" s="76"/>
+      <c r="I40" s="76"/>
+      <c r="J40" s="76"/>
+      <c r="K40" s="76"/>
+      <c r="L40" s="76"/>
+      <c r="M40" s="76"/>
+      <c r="N40" s="76"/>
+      <c r="O40" s="76"/>
+      <c r="P40" s="76"/>
+      <c r="Q40" s="76"/>
+      <c r="R40" s="76"/>
+    </row>
+    <row r="41" spans="1:35" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A41" s="75" t="s">
         <v>968</v>
       </c>
-      <c r="B41" s="75"/>
-      <c r="C41" s="75"/>
-      <c r="D41" s="75"/>
-      <c r="E41" s="75"/>
-      <c r="F41" s="75"/>
-      <c r="G41" s="75"/>
-      <c r="H41" s="75"/>
-      <c r="I41" s="75"/>
-      <c r="J41" s="75"/>
-      <c r="K41" s="75"/>
-      <c r="L41" s="75"/>
-      <c r="M41" s="75"/>
-      <c r="N41" s="75"/>
-      <c r="O41" s="75"/>
-      <c r="P41" s="75"/>
-      <c r="Q41" s="75"/>
-      <c r="R41" s="75"/>
-    </row>
-    <row r="42" spans="1:35" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A42" s="83" t="s">
+      <c r="B41" s="76"/>
+      <c r="C41" s="76"/>
+      <c r="D41" s="76"/>
+      <c r="E41" s="76"/>
+      <c r="F41" s="76"/>
+      <c r="G41" s="76"/>
+      <c r="H41" s="76"/>
+      <c r="I41" s="76"/>
+      <c r="J41" s="76"/>
+      <c r="K41" s="76"/>
+      <c r="L41" s="76"/>
+      <c r="M41" s="76"/>
+      <c r="N41" s="76"/>
+      <c r="O41" s="76"/>
+      <c r="P41" s="76"/>
+      <c r="Q41" s="76"/>
+      <c r="R41" s="76"/>
+    </row>
+    <row r="42" spans="1:35" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A42" s="75" t="s">
         <v>969</v>
       </c>
-      <c r="B42" s="75"/>
-      <c r="C42" s="75"/>
-      <c r="D42" s="75"/>
-      <c r="E42" s="75"/>
-      <c r="F42" s="75"/>
-      <c r="G42" s="75"/>
-      <c r="H42" s="75"/>
-      <c r="I42" s="75"/>
-      <c r="J42" s="75"/>
-      <c r="K42" s="75"/>
-      <c r="L42" s="75"/>
-      <c r="M42" s="75"/>
-      <c r="N42" s="75"/>
-      <c r="O42" s="75"/>
-      <c r="P42" s="75"/>
-      <c r="Q42" s="75"/>
-      <c r="R42" s="75"/>
-    </row>
-    <row r="43" spans="1:35" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A43" s="74" t="s">
+      <c r="B42" s="76"/>
+      <c r="C42" s="76"/>
+      <c r="D42" s="76"/>
+      <c r="E42" s="76"/>
+      <c r="F42" s="76"/>
+      <c r="G42" s="76"/>
+      <c r="H42" s="76"/>
+      <c r="I42" s="76"/>
+      <c r="J42" s="76"/>
+      <c r="K42" s="76"/>
+      <c r="L42" s="76"/>
+      <c r="M42" s="76"/>
+      <c r="N42" s="76"/>
+      <c r="O42" s="76"/>
+      <c r="P42" s="76"/>
+      <c r="Q42" s="76"/>
+      <c r="R42" s="76"/>
+    </row>
+    <row r="43" spans="1:35" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A43" s="77" t="s">
         <v>970</v>
       </c>
-      <c r="B43" s="75"/>
-      <c r="C43" s="75"/>
-      <c r="D43" s="75"/>
-      <c r="E43" s="75"/>
-      <c r="F43" s="75"/>
-      <c r="G43" s="75"/>
-      <c r="H43" s="75"/>
-      <c r="I43" s="75"/>
-      <c r="J43" s="75"/>
-      <c r="K43" s="75"/>
-      <c r="L43" s="75"/>
-      <c r="M43" s="75"/>
-      <c r="N43" s="75"/>
-      <c r="O43" s="75"/>
-      <c r="P43" s="75"/>
-      <c r="Q43" s="75"/>
-      <c r="R43" s="75"/>
-    </row>
-    <row r="44" spans="1:35" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A44" s="74" t="s">
+      <c r="B43" s="76"/>
+      <c r="C43" s="76"/>
+      <c r="D43" s="76"/>
+      <c r="E43" s="76"/>
+      <c r="F43" s="76"/>
+      <c r="G43" s="76"/>
+      <c r="H43" s="76"/>
+      <c r="I43" s="76"/>
+      <c r="J43" s="76"/>
+      <c r="K43" s="76"/>
+      <c r="L43" s="76"/>
+      <c r="M43" s="76"/>
+      <c r="N43" s="76"/>
+      <c r="O43" s="76"/>
+      <c r="P43" s="76"/>
+      <c r="Q43" s="76"/>
+      <c r="R43" s="76"/>
+    </row>
+    <row r="44" spans="1:35" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A44" s="77" t="s">
         <v>971</v>
       </c>
-      <c r="B44" s="75"/>
-      <c r="C44" s="75"/>
-      <c r="D44" s="75"/>
-      <c r="E44" s="75"/>
-      <c r="F44" s="75"/>
-      <c r="G44" s="75"/>
-      <c r="H44" s="75"/>
-      <c r="I44" s="75"/>
-      <c r="J44" s="75"/>
-      <c r="K44" s="75"/>
-      <c r="L44" s="75"/>
-      <c r="M44" s="75"/>
-      <c r="N44" s="75"/>
-      <c r="O44" s="75"/>
-      <c r="P44" s="75"/>
-      <c r="Q44" s="75"/>
-      <c r="R44" s="75"/>
-    </row>
-    <row r="45" spans="1:35" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A45" s="95" t="s">
+      <c r="B44" s="76"/>
+      <c r="C44" s="76"/>
+      <c r="D44" s="76"/>
+      <c r="E44" s="76"/>
+      <c r="F44" s="76"/>
+      <c r="G44" s="76"/>
+      <c r="H44" s="76"/>
+      <c r="I44" s="76"/>
+      <c r="J44" s="76"/>
+      <c r="K44" s="76"/>
+      <c r="L44" s="76"/>
+      <c r="M44" s="76"/>
+      <c r="N44" s="76"/>
+      <c r="O44" s="76"/>
+      <c r="P44" s="76"/>
+      <c r="Q44" s="76"/>
+      <c r="R44" s="76"/>
+    </row>
+    <row r="45" spans="1:35" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A45" s="78" t="s">
         <v>972</v>
       </c>
-      <c r="B45" s="75"/>
-      <c r="C45" s="75"/>
-      <c r="D45" s="75"/>
-      <c r="E45" s="75"/>
-      <c r="F45" s="75"/>
-      <c r="G45" s="75"/>
-      <c r="H45" s="75"/>
-      <c r="I45" s="75"/>
-      <c r="J45" s="75"/>
-      <c r="K45" s="75"/>
-      <c r="L45" s="75"/>
-      <c r="M45" s="75"/>
-      <c r="N45" s="75"/>
-      <c r="O45" s="75"/>
-      <c r="P45" s="75"/>
-      <c r="Q45" s="75"/>
-      <c r="R45" s="75"/>
-    </row>
-    <row r="46" spans="1:35" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A46" s="83" t="s">
+      <c r="B45" s="76"/>
+      <c r="C45" s="76"/>
+      <c r="D45" s="76"/>
+      <c r="E45" s="76"/>
+      <c r="F45" s="76"/>
+      <c r="G45" s="76"/>
+      <c r="H45" s="76"/>
+      <c r="I45" s="76"/>
+      <c r="J45" s="76"/>
+      <c r="K45" s="76"/>
+      <c r="L45" s="76"/>
+      <c r="M45" s="76"/>
+      <c r="N45" s="76"/>
+      <c r="O45" s="76"/>
+      <c r="P45" s="76"/>
+      <c r="Q45" s="76"/>
+      <c r="R45" s="76"/>
+    </row>
+    <row r="46" spans="1:35" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A46" s="75" t="s">
         <v>973</v>
       </c>
-      <c r="B46" s="75"/>
-      <c r="C46" s="75"/>
-      <c r="D46" s="75"/>
-      <c r="E46" s="75"/>
-      <c r="F46" s="75"/>
-      <c r="G46" s="75"/>
-      <c r="H46" s="75"/>
-      <c r="I46" s="75"/>
-      <c r="J46" s="75"/>
-      <c r="K46" s="75"/>
-      <c r="L46" s="75"/>
-      <c r="M46" s="75"/>
-      <c r="N46" s="75"/>
-      <c r="O46" s="75"/>
-      <c r="P46" s="75"/>
-      <c r="Q46" s="75"/>
-      <c r="R46" s="75"/>
-    </row>
-    <row r="47" spans="1:35" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A47" s="83" t="s">
+      <c r="B46" s="76"/>
+      <c r="C46" s="76"/>
+      <c r="D46" s="76"/>
+      <c r="E46" s="76"/>
+      <c r="F46" s="76"/>
+      <c r="G46" s="76"/>
+      <c r="H46" s="76"/>
+      <c r="I46" s="76"/>
+      <c r="J46" s="76"/>
+      <c r="K46" s="76"/>
+      <c r="L46" s="76"/>
+      <c r="M46" s="76"/>
+      <c r="N46" s="76"/>
+      <c r="O46" s="76"/>
+      <c r="P46" s="76"/>
+      <c r="Q46" s="76"/>
+      <c r="R46" s="76"/>
+    </row>
+    <row r="47" spans="1:35" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A47" s="75" t="s">
         <v>974</v>
       </c>
-      <c r="B47" s="75"/>
-      <c r="C47" s="75"/>
-      <c r="D47" s="75"/>
-      <c r="E47" s="75"/>
-      <c r="F47" s="75"/>
-      <c r="G47" s="75"/>
-      <c r="H47" s="75"/>
-      <c r="I47" s="75"/>
-      <c r="J47" s="75"/>
-      <c r="K47" s="75"/>
-      <c r="L47" s="75"/>
-      <c r="M47" s="75"/>
-      <c r="N47" s="75"/>
-      <c r="O47" s="75"/>
-      <c r="P47" s="75"/>
-      <c r="Q47" s="75"/>
-      <c r="R47" s="75"/>
-    </row>
-    <row r="48" spans="1:35" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A48" s="83" t="s">
+      <c r="B47" s="76"/>
+      <c r="C47" s="76"/>
+      <c r="D47" s="76"/>
+      <c r="E47" s="76"/>
+      <c r="F47" s="76"/>
+      <c r="G47" s="76"/>
+      <c r="H47" s="76"/>
+      <c r="I47" s="76"/>
+      <c r="J47" s="76"/>
+      <c r="K47" s="76"/>
+      <c r="L47" s="76"/>
+      <c r="M47" s="76"/>
+      <c r="N47" s="76"/>
+      <c r="O47" s="76"/>
+      <c r="P47" s="76"/>
+      <c r="Q47" s="76"/>
+      <c r="R47" s="76"/>
+    </row>
+    <row r="48" spans="1:35" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A48" s="75" t="s">
         <v>975</v>
       </c>
-      <c r="B48" s="75"/>
-      <c r="C48" s="75"/>
-      <c r="D48" s="75"/>
-      <c r="E48" s="75"/>
-      <c r="F48" s="75"/>
-      <c r="G48" s="75"/>
-      <c r="H48" s="75"/>
-      <c r="I48" s="75"/>
-      <c r="J48" s="75"/>
-      <c r="K48" s="75"/>
-      <c r="L48" s="75"/>
-      <c r="M48" s="75"/>
-      <c r="N48" s="75"/>
-      <c r="O48" s="75"/>
-      <c r="P48" s="75"/>
-      <c r="Q48" s="75"/>
-      <c r="R48" s="75"/>
-    </row>
-    <row r="49" spans="1:18" s="68" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A49" s="83" t="s">
+      <c r="B48" s="76"/>
+      <c r="C48" s="76"/>
+      <c r="D48" s="76"/>
+      <c r="E48" s="76"/>
+      <c r="F48" s="76"/>
+      <c r="G48" s="76"/>
+      <c r="H48" s="76"/>
+      <c r="I48" s="76"/>
+      <c r="J48" s="76"/>
+      <c r="K48" s="76"/>
+      <c r="L48" s="76"/>
+      <c r="M48" s="76"/>
+      <c r="N48" s="76"/>
+      <c r="O48" s="76"/>
+      <c r="P48" s="76"/>
+      <c r="Q48" s="76"/>
+      <c r="R48" s="76"/>
+    </row>
+    <row r="49" spans="1:18" s="70" customFormat="1" ht="25.5" customHeight="1">
+      <c r="A49" s="75" t="s">
         <v>976</v>
       </c>
-      <c r="B49" s="75"/>
-      <c r="C49" s="75"/>
-      <c r="D49" s="75"/>
-      <c r="E49" s="75"/>
-      <c r="F49" s="75"/>
-      <c r="G49" s="75"/>
-      <c r="H49" s="75"/>
-      <c r="I49" s="75"/>
-      <c r="J49" s="75"/>
-      <c r="K49" s="75"/>
-      <c r="L49" s="75"/>
-      <c r="M49" s="75"/>
-      <c r="N49" s="75"/>
-      <c r="O49" s="75"/>
-      <c r="P49" s="75"/>
-      <c r="Q49" s="75"/>
-      <c r="R49" s="75"/>
-    </row>
-    <row r="50" spans="1:18" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A50" s="83" t="s">
+      <c r="B49" s="76"/>
+      <c r="C49" s="76"/>
+      <c r="D49" s="76"/>
+      <c r="E49" s="76"/>
+      <c r="F49" s="76"/>
+      <c r="G49" s="76"/>
+      <c r="H49" s="76"/>
+      <c r="I49" s="76"/>
+      <c r="J49" s="76"/>
+      <c r="K49" s="76"/>
+      <c r="L49" s="76"/>
+      <c r="M49" s="76"/>
+      <c r="N49" s="76"/>
+      <c r="O49" s="76"/>
+      <c r="P49" s="76"/>
+      <c r="Q49" s="76"/>
+      <c r="R49" s="76"/>
+    </row>
+    <row r="50" spans="1:18" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A50" s="75" t="s">
         <v>977</v>
       </c>
-      <c r="B50" s="75"/>
-      <c r="C50" s="75"/>
-      <c r="D50" s="75"/>
-      <c r="E50" s="75"/>
-      <c r="F50" s="75"/>
-      <c r="G50" s="75"/>
-      <c r="H50" s="75"/>
-      <c r="I50" s="75"/>
-      <c r="J50" s="75"/>
-      <c r="K50" s="75"/>
-      <c r="L50" s="75"/>
-      <c r="M50" s="75"/>
-      <c r="N50" s="75"/>
-      <c r="O50" s="75"/>
-      <c r="P50" s="75"/>
-    </row>
-    <row r="51" spans="1:18" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A51" s="76"/>
-      <c r="B51" s="75"/>
-      <c r="C51" s="75"/>
-      <c r="D51" s="75"/>
-      <c r="E51" s="75"/>
-      <c r="F51" s="75"/>
-      <c r="G51" s="75"/>
-      <c r="H51" s="75"/>
-      <c r="I51" s="75"/>
-      <c r="J51" s="75"/>
-      <c r="K51" s="75"/>
-      <c r="L51" s="75"/>
-      <c r="M51" s="75"/>
-      <c r="N51" s="75"/>
-      <c r="O51" s="75"/>
-      <c r="P51" s="75"/>
-    </row>
-    <row r="52" spans="1:18" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A52" s="94" t="s">
+      <c r="B50" s="76"/>
+      <c r="C50" s="76"/>
+      <c r="D50" s="76"/>
+      <c r="E50" s="76"/>
+      <c r="F50" s="76"/>
+      <c r="G50" s="76"/>
+      <c r="H50" s="76"/>
+      <c r="I50" s="76"/>
+      <c r="J50" s="76"/>
+      <c r="K50" s="76"/>
+      <c r="L50" s="76"/>
+      <c r="M50" s="76"/>
+      <c r="N50" s="76"/>
+      <c r="O50" s="76"/>
+      <c r="P50" s="76"/>
+    </row>
+    <row r="51" spans="1:18" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A51" s="98"/>
+      <c r="B51" s="76"/>
+      <c r="C51" s="76"/>
+      <c r="D51" s="76"/>
+      <c r="E51" s="76"/>
+      <c r="F51" s="76"/>
+      <c r="G51" s="76"/>
+      <c r="H51" s="76"/>
+      <c r="I51" s="76"/>
+      <c r="J51" s="76"/>
+      <c r="K51" s="76"/>
+      <c r="L51" s="76"/>
+      <c r="M51" s="76"/>
+      <c r="N51" s="76"/>
+      <c r="O51" s="76"/>
+      <c r="P51" s="76"/>
+    </row>
+    <row r="52" spans="1:18" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A52" s="87" t="s">
         <v>978</v>
       </c>
-      <c r="B52" s="75"/>
-      <c r="C52" s="75"/>
-      <c r="D52" s="75"/>
-      <c r="E52" s="75"/>
-      <c r="F52" s="75"/>
-      <c r="G52" s="75"/>
-      <c r="H52" s="75"/>
-      <c r="I52" s="75"/>
-      <c r="J52" s="75"/>
-      <c r="K52" s="75"/>
-      <c r="L52" s="75"/>
-      <c r="M52" s="75"/>
-      <c r="N52" s="75"/>
-      <c r="O52" s="75"/>
-      <c r="P52" s="75"/>
-    </row>
-    <row r="53" spans="1:18" s="68" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A53" s="95" t="s">
+      <c r="B52" s="76"/>
+      <c r="C52" s="76"/>
+      <c r="D52" s="76"/>
+      <c r="E52" s="76"/>
+      <c r="F52" s="76"/>
+      <c r="G52" s="76"/>
+      <c r="H52" s="76"/>
+      <c r="I52" s="76"/>
+      <c r="J52" s="76"/>
+      <c r="K52" s="76"/>
+      <c r="L52" s="76"/>
+      <c r="M52" s="76"/>
+      <c r="N52" s="76"/>
+      <c r="O52" s="76"/>
+      <c r="P52" s="76"/>
+    </row>
+    <row r="53" spans="1:18" s="70" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A53" s="78" t="s">
         <v>979</v>
       </c>
-      <c r="B53" s="75"/>
-      <c r="C53" s="75"/>
-      <c r="D53" s="75"/>
-      <c r="E53" s="75"/>
-      <c r="F53" s="75"/>
-      <c r="G53" s="75"/>
-      <c r="H53" s="75"/>
-      <c r="I53" s="75"/>
-      <c r="J53" s="75"/>
-      <c r="K53" s="75"/>
-      <c r="L53" s="75"/>
-      <c r="M53" s="75"/>
-      <c r="N53" s="75"/>
-      <c r="O53" s="75"/>
-      <c r="P53" s="75"/>
-    </row>
-    <row r="54" spans="1:18" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A54" s="77" t="s">
+      <c r="B53" s="76"/>
+      <c r="C53" s="76"/>
+      <c r="D53" s="76"/>
+      <c r="E53" s="76"/>
+      <c r="F53" s="76"/>
+      <c r="G53" s="76"/>
+      <c r="H53" s="76"/>
+      <c r="I53" s="76"/>
+      <c r="J53" s="76"/>
+      <c r="K53" s="76"/>
+      <c r="L53" s="76"/>
+      <c r="M53" s="76"/>
+      <c r="N53" s="76"/>
+      <c r="O53" s="76"/>
+      <c r="P53" s="76"/>
+    </row>
+    <row r="54" spans="1:18" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A54" s="80" t="s">
         <v>980</v>
       </c>
-      <c r="B54" s="75"/>
-      <c r="C54" s="75"/>
-      <c r="D54" s="75"/>
-      <c r="E54" s="75"/>
-      <c r="F54" s="75"/>
-      <c r="G54" s="75"/>
-      <c r="H54" s="75"/>
-      <c r="I54" s="75"/>
-      <c r="J54" s="75"/>
-      <c r="K54" s="75"/>
-      <c r="L54" s="75"/>
-      <c r="M54" s="75"/>
-      <c r="N54" s="75"/>
-      <c r="O54" s="75"/>
-      <c r="P54" s="75"/>
-    </row>
-    <row r="55" spans="1:18" s="68" customFormat="1" ht="38.25" customHeight="1">
-      <c r="A55" s="79" t="s">
+      <c r="B54" s="76"/>
+      <c r="C54" s="76"/>
+      <c r="D54" s="76"/>
+      <c r="E54" s="76"/>
+      <c r="F54" s="76"/>
+      <c r="G54" s="76"/>
+      <c r="H54" s="76"/>
+      <c r="I54" s="76"/>
+      <c r="J54" s="76"/>
+      <c r="K54" s="76"/>
+      <c r="L54" s="76"/>
+      <c r="M54" s="76"/>
+      <c r="N54" s="76"/>
+      <c r="O54" s="76"/>
+      <c r="P54" s="76"/>
+    </row>
+    <row r="55" spans="1:18" s="70" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A55" s="99" t="s">
         <v>981</v>
       </c>
-      <c r="B55" s="75"/>
-      <c r="C55" s="75"/>
-      <c r="D55" s="75"/>
-      <c r="E55" s="75"/>
-      <c r="F55" s="75"/>
-      <c r="G55" s="75"/>
-      <c r="H55" s="75"/>
-      <c r="I55" s="75"/>
-      <c r="J55" s="75"/>
-      <c r="K55" s="75"/>
-      <c r="L55" s="75"/>
-      <c r="M55" s="75"/>
-      <c r="N55" s="75"/>
-      <c r="O55" s="75"/>
-      <c r="P55" s="75"/>
-    </row>
-    <row r="56" spans="1:18" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A56" s="77" t="s">
+      <c r="B55" s="76"/>
+      <c r="C55" s="76"/>
+      <c r="D55" s="76"/>
+      <c r="E55" s="76"/>
+      <c r="F55" s="76"/>
+      <c r="G55" s="76"/>
+      <c r="H55" s="76"/>
+      <c r="I55" s="76"/>
+      <c r="J55" s="76"/>
+      <c r="K55" s="76"/>
+      <c r="L55" s="76"/>
+      <c r="M55" s="76"/>
+      <c r="N55" s="76"/>
+      <c r="O55" s="76"/>
+      <c r="P55" s="76"/>
+    </row>
+    <row r="56" spans="1:18" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A56" s="80" t="s">
         <v>982</v>
       </c>
-      <c r="B56" s="75"/>
-      <c r="C56" s="75"/>
-      <c r="D56" s="75"/>
-      <c r="E56" s="75"/>
-      <c r="F56" s="75"/>
-      <c r="G56" s="75"/>
-      <c r="H56" s="75"/>
-      <c r="I56" s="75"/>
-      <c r="J56" s="75"/>
-      <c r="K56" s="75"/>
-      <c r="L56" s="75"/>
-      <c r="M56" s="75"/>
-      <c r="N56" s="75"/>
-      <c r="O56" s="75"/>
-      <c r="P56" s="75"/>
-    </row>
-    <row r="57" spans="1:18" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A57" s="77" t="s">
+      <c r="B56" s="76"/>
+      <c r="C56" s="76"/>
+      <c r="D56" s="76"/>
+      <c r="E56" s="76"/>
+      <c r="F56" s="76"/>
+      <c r="G56" s="76"/>
+      <c r="H56" s="76"/>
+      <c r="I56" s="76"/>
+      <c r="J56" s="76"/>
+      <c r="K56" s="76"/>
+      <c r="L56" s="76"/>
+      <c r="M56" s="76"/>
+      <c r="N56" s="76"/>
+      <c r="O56" s="76"/>
+      <c r="P56" s="76"/>
+    </row>
+    <row r="57" spans="1:18" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A57" s="80" t="s">
         <v>983</v>
       </c>
-      <c r="B57" s="75"/>
-      <c r="C57" s="75"/>
-      <c r="D57" s="75"/>
-      <c r="E57" s="75"/>
-      <c r="F57" s="75"/>
-      <c r="G57" s="75"/>
-      <c r="H57" s="75"/>
-      <c r="I57" s="75"/>
-      <c r="J57" s="75"/>
-      <c r="K57" s="75"/>
-      <c r="L57" s="75"/>
-      <c r="M57" s="75"/>
-      <c r="N57" s="75"/>
-      <c r="O57" s="75"/>
-      <c r="P57" s="75"/>
-    </row>
-    <row r="58" spans="1:18" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A58" s="96" t="s">
+      <c r="B57" s="76"/>
+      <c r="C57" s="76"/>
+      <c r="D57" s="76"/>
+      <c r="E57" s="76"/>
+      <c r="F57" s="76"/>
+      <c r="G57" s="76"/>
+      <c r="H57" s="76"/>
+      <c r="I57" s="76"/>
+      <c r="J57" s="76"/>
+      <c r="K57" s="76"/>
+      <c r="L57" s="76"/>
+      <c r="M57" s="76"/>
+      <c r="N57" s="76"/>
+      <c r="O57" s="76"/>
+      <c r="P57" s="76"/>
+    </row>
+    <row r="58" spans="1:18" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A58" s="88" t="s">
         <v>984</v>
       </c>
-      <c r="B58" s="75"/>
-      <c r="C58" s="75"/>
-      <c r="D58" s="75"/>
-      <c r="E58" s="75"/>
-      <c r="F58" s="75"/>
-      <c r="G58" s="75"/>
-      <c r="H58" s="75"/>
-      <c r="I58" s="75"/>
-      <c r="J58" s="75"/>
-      <c r="K58" s="75"/>
-      <c r="L58" s="75"/>
-      <c r="M58" s="75"/>
-      <c r="N58" s="75"/>
-      <c r="O58" s="75"/>
-      <c r="P58" s="75"/>
-    </row>
-    <row r="59" spans="1:18" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A59" s="81"/>
-      <c r="B59" s="75"/>
-      <c r="C59" s="75"/>
-      <c r="D59" s="75"/>
-      <c r="E59" s="75"/>
-      <c r="F59" s="75"/>
-      <c r="G59" s="75"/>
-      <c r="H59" s="75"/>
-      <c r="I59" s="75"/>
-      <c r="J59" s="75"/>
-      <c r="K59" s="75"/>
-      <c r="L59" s="75"/>
-      <c r="M59" s="75"/>
-      <c r="N59" s="75"/>
-      <c r="O59" s="75"/>
-      <c r="P59" s="75"/>
-    </row>
-    <row r="60" spans="1:18" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A60" s="88" t="s">
+      <c r="B58" s="76"/>
+      <c r="C58" s="76"/>
+      <c r="D58" s="76"/>
+      <c r="E58" s="76"/>
+      <c r="F58" s="76"/>
+      <c r="G58" s="76"/>
+      <c r="H58" s="76"/>
+      <c r="I58" s="76"/>
+      <c r="J58" s="76"/>
+      <c r="K58" s="76"/>
+      <c r="L58" s="76"/>
+      <c r="M58" s="76"/>
+      <c r="N58" s="76"/>
+      <c r="O58" s="76"/>
+      <c r="P58" s="76"/>
+    </row>
+    <row r="59" spans="1:18" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A59" s="100"/>
+      <c r="B59" s="76"/>
+      <c r="C59" s="76"/>
+      <c r="D59" s="76"/>
+      <c r="E59" s="76"/>
+      <c r="F59" s="76"/>
+      <c r="G59" s="76"/>
+      <c r="H59" s="76"/>
+      <c r="I59" s="76"/>
+      <c r="J59" s="76"/>
+      <c r="K59" s="76"/>
+      <c r="L59" s="76"/>
+      <c r="M59" s="76"/>
+      <c r="N59" s="76"/>
+      <c r="O59" s="76"/>
+      <c r="P59" s="76"/>
+    </row>
+    <row r="60" spans="1:18" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A60" s="89" t="s">
         <v>985</v>
       </c>
-      <c r="B60" s="75"/>
-      <c r="C60" s="75"/>
-      <c r="D60" s="75"/>
-      <c r="E60" s="75"/>
-      <c r="F60" s="75"/>
-      <c r="G60" s="75"/>
-      <c r="H60" s="75"/>
-      <c r="I60" s="75"/>
-      <c r="J60" s="75"/>
-      <c r="K60" s="75"/>
-      <c r="L60" s="75"/>
-      <c r="M60" s="75"/>
-      <c r="N60" s="75"/>
-      <c r="O60" s="75"/>
-      <c r="P60" s="75"/>
-    </row>
-    <row r="61" spans="1:18" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A61" s="88" t="s">
+      <c r="B60" s="76"/>
+      <c r="C60" s="76"/>
+      <c r="D60" s="76"/>
+      <c r="E60" s="76"/>
+      <c r="F60" s="76"/>
+      <c r="G60" s="76"/>
+      <c r="H60" s="76"/>
+      <c r="I60" s="76"/>
+      <c r="J60" s="76"/>
+      <c r="K60" s="76"/>
+      <c r="L60" s="76"/>
+      <c r="M60" s="76"/>
+      <c r="N60" s="76"/>
+      <c r="O60" s="76"/>
+      <c r="P60" s="76"/>
+    </row>
+    <row r="61" spans="1:18" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A61" s="89" t="s">
         <v>986</v>
       </c>
-      <c r="B61" s="75"/>
-      <c r="C61" s="75"/>
-      <c r="D61" s="75"/>
-      <c r="E61" s="75"/>
-      <c r="F61" s="75"/>
-      <c r="G61" s="75"/>
-      <c r="H61" s="75"/>
-      <c r="I61" s="75"/>
-      <c r="J61" s="75"/>
-      <c r="K61" s="75"/>
-      <c r="L61" s="75"/>
-      <c r="M61" s="75"/>
-      <c r="N61" s="75"/>
-      <c r="O61" s="75"/>
-      <c r="P61" s="75"/>
-    </row>
-    <row r="62" spans="1:18" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A62" s="82" t="s">
+      <c r="B61" s="76"/>
+      <c r="C61" s="76"/>
+      <c r="D61" s="76"/>
+      <c r="E61" s="76"/>
+      <c r="F61" s="76"/>
+      <c r="G61" s="76"/>
+      <c r="H61" s="76"/>
+      <c r="I61" s="76"/>
+      <c r="J61" s="76"/>
+      <c r="K61" s="76"/>
+      <c r="L61" s="76"/>
+      <c r="M61" s="76"/>
+      <c r="N61" s="76"/>
+      <c r="O61" s="76"/>
+      <c r="P61" s="76"/>
+    </row>
+    <row r="62" spans="1:18" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A62" s="83" t="s">
         <v>987</v>
       </c>
-      <c r="B62" s="75"/>
-      <c r="C62" s="75"/>
-      <c r="D62" s="75"/>
-      <c r="E62" s="75"/>
-      <c r="F62" s="75"/>
-      <c r="G62" s="75"/>
-      <c r="H62" s="75"/>
-      <c r="I62" s="75"/>
-      <c r="J62" s="75"/>
-      <c r="K62" s="75"/>
-      <c r="L62" s="75"/>
-      <c r="M62" s="75"/>
-      <c r="N62" s="75"/>
-      <c r="O62" s="75"/>
-      <c r="P62" s="75"/>
-    </row>
-    <row r="63" spans="1:18" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A63" s="97" t="s">
+      <c r="B62" s="76"/>
+      <c r="C62" s="76"/>
+      <c r="D62" s="76"/>
+      <c r="E62" s="76"/>
+      <c r="F62" s="76"/>
+      <c r="G62" s="76"/>
+      <c r="H62" s="76"/>
+      <c r="I62" s="76"/>
+      <c r="J62" s="76"/>
+      <c r="K62" s="76"/>
+      <c r="L62" s="76"/>
+      <c r="M62" s="76"/>
+      <c r="N62" s="76"/>
+      <c r="O62" s="76"/>
+      <c r="P62" s="76"/>
+    </row>
+    <row r="63" spans="1:18" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A63" s="90" t="s">
         <v>988</v>
       </c>
-      <c r="B63" s="75"/>
-      <c r="C63" s="75"/>
-      <c r="D63" s="75"/>
-      <c r="E63" s="75"/>
-      <c r="F63" s="75"/>
-      <c r="G63" s="75"/>
-      <c r="H63" s="75"/>
-      <c r="I63" s="75"/>
-      <c r="J63" s="75"/>
-      <c r="K63" s="75"/>
-      <c r="L63" s="75"/>
-      <c r="M63" s="75"/>
-      <c r="N63" s="75"/>
-      <c r="O63" s="75"/>
-      <c r="P63" s="75"/>
-    </row>
-    <row r="64" spans="1:18" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A64" s="78" t="s">
+      <c r="B63" s="76"/>
+      <c r="C63" s="76"/>
+      <c r="D63" s="76"/>
+      <c r="E63" s="76"/>
+      <c r="F63" s="76"/>
+      <c r="G63" s="76"/>
+      <c r="H63" s="76"/>
+      <c r="I63" s="76"/>
+      <c r="J63" s="76"/>
+      <c r="K63" s="76"/>
+      <c r="L63" s="76"/>
+      <c r="M63" s="76"/>
+      <c r="N63" s="76"/>
+      <c r="O63" s="76"/>
+      <c r="P63" s="76"/>
+    </row>
+    <row r="64" spans="1:18" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A64" s="79" t="s">
         <v>989</v>
       </c>
-      <c r="B64" s="75"/>
-      <c r="C64" s="75"/>
-      <c r="D64" s="75"/>
-      <c r="E64" s="75"/>
-      <c r="F64" s="75"/>
-      <c r="G64" s="75"/>
-      <c r="H64" s="75"/>
-      <c r="I64" s="75"/>
-      <c r="J64" s="75"/>
-      <c r="K64" s="75"/>
-      <c r="L64" s="75"/>
-      <c r="M64" s="75"/>
-      <c r="N64" s="75"/>
-      <c r="O64" s="75"/>
-      <c r="P64" s="75"/>
-    </row>
-    <row r="65" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A65" s="78" t="s">
+      <c r="B64" s="76"/>
+      <c r="C64" s="76"/>
+      <c r="D64" s="76"/>
+      <c r="E64" s="76"/>
+      <c r="F64" s="76"/>
+      <c r="G64" s="76"/>
+      <c r="H64" s="76"/>
+      <c r="I64" s="76"/>
+      <c r="J64" s="76"/>
+      <c r="K64" s="76"/>
+      <c r="L64" s="76"/>
+      <c r="M64" s="76"/>
+      <c r="N64" s="76"/>
+      <c r="O64" s="76"/>
+      <c r="P64" s="76"/>
+    </row>
+    <row r="65" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A65" s="79" t="s">
         <v>990</v>
       </c>
-      <c r="B65" s="75"/>
-      <c r="C65" s="75"/>
-      <c r="D65" s="75"/>
-      <c r="E65" s="75"/>
-      <c r="F65" s="75"/>
-      <c r="G65" s="75"/>
-      <c r="H65" s="75"/>
-      <c r="I65" s="75"/>
-      <c r="J65" s="75"/>
-      <c r="K65" s="75"/>
-      <c r="L65" s="75"/>
-      <c r="M65" s="75"/>
-      <c r="N65" s="75"/>
-      <c r="O65" s="75"/>
-      <c r="P65" s="75"/>
-    </row>
-    <row r="66" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A66" s="78" t="s">
+      <c r="B65" s="76"/>
+      <c r="C65" s="76"/>
+      <c r="D65" s="76"/>
+      <c r="E65" s="76"/>
+      <c r="F65" s="76"/>
+      <c r="G65" s="76"/>
+      <c r="H65" s="76"/>
+      <c r="I65" s="76"/>
+      <c r="J65" s="76"/>
+      <c r="K65" s="76"/>
+      <c r="L65" s="76"/>
+      <c r="M65" s="76"/>
+      <c r="N65" s="76"/>
+      <c r="O65" s="76"/>
+      <c r="P65" s="76"/>
+    </row>
+    <row r="66" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A66" s="79" t="s">
         <v>991</v>
       </c>
-      <c r="B66" s="75"/>
-      <c r="C66" s="75"/>
-      <c r="D66" s="75"/>
-      <c r="E66" s="75"/>
-      <c r="F66" s="75"/>
-      <c r="G66" s="75"/>
-      <c r="H66" s="75"/>
-      <c r="I66" s="75"/>
-      <c r="J66" s="75"/>
-      <c r="K66" s="75"/>
-      <c r="L66" s="75"/>
-      <c r="M66" s="75"/>
-      <c r="N66" s="75"/>
-      <c r="O66" s="75"/>
-      <c r="P66" s="75"/>
-    </row>
-    <row r="67" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A67" s="78" t="s">
+      <c r="B66" s="76"/>
+      <c r="C66" s="76"/>
+      <c r="D66" s="76"/>
+      <c r="E66" s="76"/>
+      <c r="F66" s="76"/>
+      <c r="G66" s="76"/>
+      <c r="H66" s="76"/>
+      <c r="I66" s="76"/>
+      <c r="J66" s="76"/>
+      <c r="K66" s="76"/>
+      <c r="L66" s="76"/>
+      <c r="M66" s="76"/>
+      <c r="N66" s="76"/>
+      <c r="O66" s="76"/>
+      <c r="P66" s="76"/>
+    </row>
+    <row r="67" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A67" s="79" t="s">
         <v>992</v>
       </c>
-      <c r="B67" s="75"/>
-      <c r="C67" s="75"/>
-      <c r="D67" s="75"/>
-      <c r="E67" s="75"/>
-      <c r="F67" s="75"/>
-      <c r="G67" s="75"/>
-      <c r="H67" s="75"/>
-      <c r="I67" s="75"/>
-      <c r="J67" s="75"/>
-      <c r="K67" s="75"/>
-      <c r="L67" s="75"/>
-      <c r="M67" s="75"/>
-      <c r="N67" s="75"/>
-      <c r="O67" s="75"/>
-      <c r="P67" s="75"/>
-    </row>
-    <row r="68" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A68" s="82" t="s">
+      <c r="B67" s="76"/>
+      <c r="C67" s="76"/>
+      <c r="D67" s="76"/>
+      <c r="E67" s="76"/>
+      <c r="F67" s="76"/>
+      <c r="G67" s="76"/>
+      <c r="H67" s="76"/>
+      <c r="I67" s="76"/>
+      <c r="J67" s="76"/>
+      <c r="K67" s="76"/>
+      <c r="L67" s="76"/>
+      <c r="M67" s="76"/>
+      <c r="N67" s="76"/>
+      <c r="O67" s="76"/>
+      <c r="P67" s="76"/>
+    </row>
+    <row r="68" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A68" s="83" t="s">
         <v>993</v>
       </c>
-      <c r="B68" s="75"/>
-      <c r="C68" s="75"/>
-      <c r="D68" s="75"/>
-      <c r="E68" s="75"/>
-      <c r="F68" s="75"/>
-      <c r="G68" s="75"/>
-      <c r="H68" s="75"/>
-      <c r="I68" s="75"/>
-      <c r="J68" s="75"/>
-      <c r="K68" s="75"/>
-      <c r="L68" s="75"/>
-      <c r="M68" s="75"/>
-      <c r="N68" s="75"/>
-      <c r="O68" s="75"/>
-      <c r="P68" s="75"/>
-    </row>
-    <row r="69" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A69" s="78" t="s">
+      <c r="B68" s="76"/>
+      <c r="C68" s="76"/>
+      <c r="D68" s="76"/>
+      <c r="E68" s="76"/>
+      <c r="F68" s="76"/>
+      <c r="G68" s="76"/>
+      <c r="H68" s="76"/>
+      <c r="I68" s="76"/>
+      <c r="J68" s="76"/>
+      <c r="K68" s="76"/>
+      <c r="L68" s="76"/>
+      <c r="M68" s="76"/>
+      <c r="N68" s="76"/>
+      <c r="O68" s="76"/>
+      <c r="P68" s="76"/>
+    </row>
+    <row r="69" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A69" s="79" t="s">
         <v>994</v>
       </c>
-      <c r="B69" s="75"/>
-      <c r="C69" s="75"/>
-      <c r="D69" s="75"/>
-      <c r="E69" s="75"/>
-      <c r="F69" s="75"/>
-      <c r="G69" s="75"/>
-      <c r="H69" s="75"/>
-      <c r="I69" s="75"/>
-      <c r="J69" s="75"/>
-      <c r="K69" s="75"/>
-      <c r="L69" s="75"/>
-      <c r="M69" s="75"/>
-      <c r="N69" s="75"/>
-      <c r="O69" s="75"/>
-      <c r="P69" s="75"/>
-    </row>
-    <row r="70" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A70" s="78" t="s">
+      <c r="B69" s="76"/>
+      <c r="C69" s="76"/>
+      <c r="D69" s="76"/>
+      <c r="E69" s="76"/>
+      <c r="F69" s="76"/>
+      <c r="G69" s="76"/>
+      <c r="H69" s="76"/>
+      <c r="I69" s="76"/>
+      <c r="J69" s="76"/>
+      <c r="K69" s="76"/>
+      <c r="L69" s="76"/>
+      <c r="M69" s="76"/>
+      <c r="N69" s="76"/>
+      <c r="O69" s="76"/>
+      <c r="P69" s="76"/>
+    </row>
+    <row r="70" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A70" s="79" t="s">
         <v>995</v>
       </c>
-      <c r="B70" s="75"/>
-      <c r="C70" s="75"/>
-      <c r="D70" s="75"/>
-      <c r="E70" s="75"/>
-      <c r="F70" s="75"/>
-      <c r="G70" s="75"/>
-      <c r="H70" s="75"/>
-      <c r="I70" s="75"/>
-      <c r="J70" s="75"/>
-      <c r="K70" s="75"/>
-      <c r="L70" s="75"/>
-      <c r="M70" s="75"/>
-      <c r="N70" s="75"/>
-      <c r="O70" s="75"/>
-      <c r="P70" s="75"/>
-    </row>
-    <row r="71" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A71" s="78" t="s">
+      <c r="B70" s="76"/>
+      <c r="C70" s="76"/>
+      <c r="D70" s="76"/>
+      <c r="E70" s="76"/>
+      <c r="F70" s="76"/>
+      <c r="G70" s="76"/>
+      <c r="H70" s="76"/>
+      <c r="I70" s="76"/>
+      <c r="J70" s="76"/>
+      <c r="K70" s="76"/>
+      <c r="L70" s="76"/>
+      <c r="M70" s="76"/>
+      <c r="N70" s="76"/>
+      <c r="O70" s="76"/>
+      <c r="P70" s="76"/>
+    </row>
+    <row r="71" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A71" s="79" t="s">
         <v>996</v>
       </c>
-      <c r="B71" s="75"/>
-      <c r="C71" s="75"/>
-      <c r="D71" s="75"/>
-      <c r="E71" s="75"/>
-      <c r="F71" s="75"/>
-      <c r="G71" s="75"/>
-      <c r="H71" s="75"/>
-      <c r="I71" s="75"/>
-      <c r="J71" s="75"/>
-      <c r="K71" s="75"/>
-      <c r="L71" s="75"/>
-      <c r="M71" s="75"/>
-      <c r="N71" s="75"/>
-      <c r="O71" s="75"/>
-      <c r="P71" s="75"/>
-    </row>
-    <row r="72" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A72" s="78" t="s">
+      <c r="B71" s="76"/>
+      <c r="C71" s="76"/>
+      <c r="D71" s="76"/>
+      <c r="E71" s="76"/>
+      <c r="F71" s="76"/>
+      <c r="G71" s="76"/>
+      <c r="H71" s="76"/>
+      <c r="I71" s="76"/>
+      <c r="J71" s="76"/>
+      <c r="K71" s="76"/>
+      <c r="L71" s="76"/>
+      <c r="M71" s="76"/>
+      <c r="N71" s="76"/>
+      <c r="O71" s="76"/>
+      <c r="P71" s="76"/>
+    </row>
+    <row r="72" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A72" s="79" t="s">
         <v>997</v>
       </c>
-      <c r="B72" s="75"/>
-      <c r="C72" s="75"/>
-      <c r="D72" s="75"/>
-      <c r="E72" s="75"/>
-      <c r="F72" s="75"/>
-      <c r="G72" s="75"/>
-      <c r="H72" s="75"/>
-      <c r="I72" s="75"/>
-      <c r="J72" s="75"/>
-      <c r="K72" s="75"/>
-      <c r="L72" s="75"/>
-      <c r="M72" s="75"/>
-      <c r="N72" s="75"/>
-      <c r="O72" s="75"/>
-      <c r="P72" s="75"/>
-    </row>
-    <row r="73" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A73" s="78" t="s">
+      <c r="B72" s="76"/>
+      <c r="C72" s="76"/>
+      <c r="D72" s="76"/>
+      <c r="E72" s="76"/>
+      <c r="F72" s="76"/>
+      <c r="G72" s="76"/>
+      <c r="H72" s="76"/>
+      <c r="I72" s="76"/>
+      <c r="J72" s="76"/>
+      <c r="K72" s="76"/>
+      <c r="L72" s="76"/>
+      <c r="M72" s="76"/>
+      <c r="N72" s="76"/>
+      <c r="O72" s="76"/>
+      <c r="P72" s="76"/>
+    </row>
+    <row r="73" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A73" s="79" t="s">
         <v>998</v>
       </c>
-      <c r="B73" s="75"/>
-      <c r="C73" s="75"/>
-      <c r="D73" s="75"/>
-      <c r="E73" s="75"/>
-      <c r="F73" s="75"/>
-      <c r="G73" s="75"/>
-      <c r="H73" s="75"/>
-      <c r="I73" s="75"/>
-      <c r="J73" s="75"/>
-      <c r="K73" s="75"/>
-      <c r="L73" s="75"/>
-      <c r="M73" s="75"/>
-      <c r="N73" s="75"/>
-      <c r="O73" s="75"/>
-      <c r="P73" s="75"/>
-    </row>
-    <row r="74" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A74" s="80" t="s">
+      <c r="B73" s="76"/>
+      <c r="C73" s="76"/>
+      <c r="D73" s="76"/>
+      <c r="E73" s="76"/>
+      <c r="F73" s="76"/>
+      <c r="G73" s="76"/>
+      <c r="H73" s="76"/>
+      <c r="I73" s="76"/>
+      <c r="J73" s="76"/>
+      <c r="K73" s="76"/>
+      <c r="L73" s="76"/>
+      <c r="M73" s="76"/>
+      <c r="N73" s="76"/>
+      <c r="O73" s="76"/>
+      <c r="P73" s="76"/>
+    </row>
+    <row r="74" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A74" s="85" t="s">
         <v>999</v>
       </c>
-      <c r="B74" s="75"/>
-      <c r="C74" s="75"/>
-      <c r="D74" s="75"/>
-      <c r="E74" s="75"/>
-      <c r="F74" s="75"/>
-      <c r="G74" s="75"/>
-      <c r="H74" s="75"/>
-      <c r="I74" s="75"/>
-      <c r="J74" s="75"/>
-      <c r="K74" s="75"/>
-      <c r="L74" s="75"/>
-      <c r="M74" s="75"/>
-      <c r="N74" s="75"/>
-      <c r="O74" s="75"/>
-      <c r="P74" s="75"/>
-    </row>
-    <row r="75" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A75" s="82" t="s">
+      <c r="B74" s="76"/>
+      <c r="C74" s="76"/>
+      <c r="D74" s="76"/>
+      <c r="E74" s="76"/>
+      <c r="F74" s="76"/>
+      <c r="G74" s="76"/>
+      <c r="H74" s="76"/>
+      <c r="I74" s="76"/>
+      <c r="J74" s="76"/>
+      <c r="K74" s="76"/>
+      <c r="L74" s="76"/>
+      <c r="M74" s="76"/>
+      <c r="N74" s="76"/>
+      <c r="O74" s="76"/>
+      <c r="P74" s="76"/>
+    </row>
+    <row r="75" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A75" s="83" t="s">
         <v>1000</v>
       </c>
-      <c r="B75" s="75"/>
-      <c r="C75" s="75"/>
-      <c r="D75" s="75"/>
-      <c r="E75" s="75"/>
-      <c r="F75" s="75"/>
-      <c r="G75" s="75"/>
-      <c r="H75" s="75"/>
-      <c r="I75" s="75"/>
-      <c r="J75" s="75"/>
-      <c r="K75" s="75"/>
-      <c r="L75" s="75"/>
-      <c r="M75" s="75"/>
-      <c r="N75" s="75"/>
-      <c r="O75" s="75"/>
-      <c r="P75" s="75"/>
-    </row>
-    <row r="76" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A76" s="77" t="s">
+      <c r="B75" s="76"/>
+      <c r="C75" s="76"/>
+      <c r="D75" s="76"/>
+      <c r="E75" s="76"/>
+      <c r="F75" s="76"/>
+      <c r="G75" s="76"/>
+      <c r="H75" s="76"/>
+      <c r="I75" s="76"/>
+      <c r="J75" s="76"/>
+      <c r="K75" s="76"/>
+      <c r="L75" s="76"/>
+      <c r="M75" s="76"/>
+      <c r="N75" s="76"/>
+      <c r="O75" s="76"/>
+      <c r="P75" s="76"/>
+    </row>
+    <row r="76" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A76" s="80" t="s">
         <v>1001</v>
       </c>
-      <c r="B76" s="75"/>
-      <c r="C76" s="75"/>
-      <c r="D76" s="75"/>
-      <c r="E76" s="75"/>
-      <c r="F76" s="75"/>
-      <c r="G76" s="75"/>
-      <c r="H76" s="75"/>
-      <c r="I76" s="75"/>
-      <c r="J76" s="75"/>
-      <c r="K76" s="75"/>
-      <c r="L76" s="75"/>
-      <c r="M76" s="75"/>
-      <c r="N76" s="75"/>
-      <c r="O76" s="75"/>
-      <c r="P76" s="75"/>
-    </row>
-    <row r="77" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A77" s="93" t="s">
+      <c r="B76" s="76"/>
+      <c r="C76" s="76"/>
+      <c r="D76" s="76"/>
+      <c r="E76" s="76"/>
+      <c r="F76" s="76"/>
+      <c r="G76" s="76"/>
+      <c r="H76" s="76"/>
+      <c r="I76" s="76"/>
+      <c r="J76" s="76"/>
+      <c r="K76" s="76"/>
+      <c r="L76" s="76"/>
+      <c r="M76" s="76"/>
+      <c r="N76" s="76"/>
+      <c r="O76" s="76"/>
+      <c r="P76" s="76"/>
+    </row>
+    <row r="77" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A77" s="84" t="s">
         <v>1002</v>
       </c>
-      <c r="B77" s="75"/>
-      <c r="C77" s="75"/>
-      <c r="D77" s="75"/>
-      <c r="E77" s="75"/>
-      <c r="F77" s="75"/>
-      <c r="G77" s="75"/>
-      <c r="H77" s="75"/>
-      <c r="I77" s="75"/>
-      <c r="J77" s="75"/>
-      <c r="K77" s="75"/>
-      <c r="L77" s="75"/>
-      <c r="M77" s="75"/>
-      <c r="N77" s="75"/>
-      <c r="O77" s="75"/>
-      <c r="P77" s="75"/>
-    </row>
-    <row r="78" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A78" s="92" t="s">
+      <c r="B77" s="76"/>
+      <c r="C77" s="76"/>
+      <c r="D77" s="76"/>
+      <c r="E77" s="76"/>
+      <c r="F77" s="76"/>
+      <c r="G77" s="76"/>
+      <c r="H77" s="76"/>
+      <c r="I77" s="76"/>
+      <c r="J77" s="76"/>
+      <c r="K77" s="76"/>
+      <c r="L77" s="76"/>
+      <c r="M77" s="76"/>
+      <c r="N77" s="76"/>
+      <c r="O77" s="76"/>
+      <c r="P77" s="76"/>
+    </row>
+    <row r="78" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A78" s="86" t="s">
         <v>1003</v>
       </c>
-      <c r="B78" s="75"/>
-      <c r="C78" s="75"/>
-      <c r="D78" s="75"/>
-      <c r="E78" s="75"/>
-      <c r="F78" s="75"/>
-      <c r="G78" s="75"/>
-      <c r="H78" s="75"/>
-      <c r="I78" s="75"/>
-      <c r="J78" s="75"/>
-      <c r="K78" s="75"/>
-      <c r="L78" s="75"/>
-      <c r="M78" s="75"/>
-      <c r="N78" s="75"/>
-      <c r="O78" s="75"/>
-      <c r="P78" s="75"/>
-    </row>
-    <row r="79" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A79" s="93" t="s">
+      <c r="B78" s="76"/>
+      <c r="C78" s="76"/>
+      <c r="D78" s="76"/>
+      <c r="E78" s="76"/>
+      <c r="F78" s="76"/>
+      <c r="G78" s="76"/>
+      <c r="H78" s="76"/>
+      <c r="I78" s="76"/>
+      <c r="J78" s="76"/>
+      <c r="K78" s="76"/>
+      <c r="L78" s="76"/>
+      <c r="M78" s="76"/>
+      <c r="N78" s="76"/>
+      <c r="O78" s="76"/>
+      <c r="P78" s="76"/>
+    </row>
+    <row r="79" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A79" s="84" t="s">
         <v>1004</v>
       </c>
-      <c r="B79" s="75"/>
-      <c r="C79" s="75"/>
-      <c r="D79" s="75"/>
-      <c r="E79" s="75"/>
-      <c r="F79" s="75"/>
-      <c r="G79" s="75"/>
-      <c r="H79" s="75"/>
-      <c r="I79" s="75"/>
-      <c r="J79" s="75"/>
-      <c r="K79" s="75"/>
-      <c r="L79" s="75"/>
-      <c r="M79" s="75"/>
-      <c r="N79" s="75"/>
-      <c r="O79" s="75"/>
-      <c r="P79" s="75"/>
-    </row>
-    <row r="80" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A80" s="82" t="s">
+      <c r="B79" s="76"/>
+      <c r="C79" s="76"/>
+      <c r="D79" s="76"/>
+      <c r="E79" s="76"/>
+      <c r="F79" s="76"/>
+      <c r="G79" s="76"/>
+      <c r="H79" s="76"/>
+      <c r="I79" s="76"/>
+      <c r="J79" s="76"/>
+      <c r="K79" s="76"/>
+      <c r="L79" s="76"/>
+      <c r="M79" s="76"/>
+      <c r="N79" s="76"/>
+      <c r="O79" s="76"/>
+      <c r="P79" s="76"/>
+    </row>
+    <row r="80" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A80" s="83" t="s">
         <v>1005</v>
       </c>
-      <c r="B80" s="75"/>
-      <c r="C80" s="75"/>
-      <c r="D80" s="75"/>
-      <c r="E80" s="75"/>
-      <c r="F80" s="75"/>
-      <c r="G80" s="75"/>
-      <c r="H80" s="75"/>
-      <c r="I80" s="75"/>
-      <c r="J80" s="75"/>
-      <c r="K80" s="75"/>
-      <c r="L80" s="75"/>
-      <c r="M80" s="75"/>
-      <c r="N80" s="75"/>
-      <c r="O80" s="75"/>
-      <c r="P80" s="75"/>
-    </row>
-    <row r="81" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A81" s="77" t="s">
+      <c r="B80" s="76"/>
+      <c r="C80" s="76"/>
+      <c r="D80" s="76"/>
+      <c r="E80" s="76"/>
+      <c r="F80" s="76"/>
+      <c r="G80" s="76"/>
+      <c r="H80" s="76"/>
+      <c r="I80" s="76"/>
+      <c r="J80" s="76"/>
+      <c r="K80" s="76"/>
+      <c r="L80" s="76"/>
+      <c r="M80" s="76"/>
+      <c r="N80" s="76"/>
+      <c r="O80" s="76"/>
+      <c r="P80" s="76"/>
+    </row>
+    <row r="81" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A81" s="80" t="s">
         <v>1006</v>
       </c>
-      <c r="B81" s="75"/>
-      <c r="C81" s="75"/>
-      <c r="D81" s="75"/>
-      <c r="E81" s="75"/>
-      <c r="F81" s="75"/>
-      <c r="G81" s="75"/>
-      <c r="H81" s="75"/>
-      <c r="I81" s="75"/>
-      <c r="J81" s="75"/>
-      <c r="K81" s="75"/>
-      <c r="L81" s="75"/>
-      <c r="M81" s="75"/>
-      <c r="N81" s="75"/>
-      <c r="O81" s="75"/>
-      <c r="P81" s="75"/>
-    </row>
-    <row r="82" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A82" s="93" t="s">
+      <c r="B81" s="76"/>
+      <c r="C81" s="76"/>
+      <c r="D81" s="76"/>
+      <c r="E81" s="76"/>
+      <c r="F81" s="76"/>
+      <c r="G81" s="76"/>
+      <c r="H81" s="76"/>
+      <c r="I81" s="76"/>
+      <c r="J81" s="76"/>
+      <c r="K81" s="76"/>
+      <c r="L81" s="76"/>
+      <c r="M81" s="76"/>
+      <c r="N81" s="76"/>
+      <c r="O81" s="76"/>
+      <c r="P81" s="76"/>
+    </row>
+    <row r="82" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A82" s="84" t="s">
         <v>1007</v>
       </c>
-      <c r="B82" s="75"/>
-      <c r="C82" s="75"/>
-      <c r="D82" s="75"/>
-      <c r="E82" s="75"/>
-      <c r="F82" s="75"/>
-      <c r="G82" s="75"/>
-      <c r="H82" s="75"/>
-      <c r="I82" s="75"/>
-      <c r="J82" s="75"/>
-      <c r="K82" s="75"/>
-      <c r="L82" s="75"/>
-      <c r="M82" s="75"/>
-      <c r="N82" s="75"/>
-      <c r="O82" s="75"/>
-      <c r="P82" s="75"/>
-    </row>
-    <row r="83" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A83" s="82" t="s">
+      <c r="B82" s="76"/>
+      <c r="C82" s="76"/>
+      <c r="D82" s="76"/>
+      <c r="E82" s="76"/>
+      <c r="F82" s="76"/>
+      <c r="G82" s="76"/>
+      <c r="H82" s="76"/>
+      <c r="I82" s="76"/>
+      <c r="J82" s="76"/>
+      <c r="K82" s="76"/>
+      <c r="L82" s="76"/>
+      <c r="M82" s="76"/>
+      <c r="N82" s="76"/>
+      <c r="O82" s="76"/>
+      <c r="P82" s="76"/>
+    </row>
+    <row r="83" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A83" s="83" t="s">
         <v>1008</v>
       </c>
-      <c r="B83" s="75"/>
-      <c r="C83" s="75"/>
-      <c r="D83" s="75"/>
-      <c r="E83" s="75"/>
-      <c r="F83" s="75"/>
-      <c r="G83" s="75"/>
-      <c r="H83" s="75"/>
-      <c r="I83" s="75"/>
-      <c r="J83" s="75"/>
-      <c r="K83" s="75"/>
-      <c r="L83" s="75"/>
-      <c r="M83" s="75"/>
-      <c r="N83" s="75"/>
-      <c r="O83" s="75"/>
-      <c r="P83" s="75"/>
-    </row>
-    <row r="84" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A84" s="77" t="s">
+      <c r="B83" s="76"/>
+      <c r="C83" s="76"/>
+      <c r="D83" s="76"/>
+      <c r="E83" s="76"/>
+      <c r="F83" s="76"/>
+      <c r="G83" s="76"/>
+      <c r="H83" s="76"/>
+      <c r="I83" s="76"/>
+      <c r="J83" s="76"/>
+      <c r="K83" s="76"/>
+      <c r="L83" s="76"/>
+      <c r="M83" s="76"/>
+      <c r="N83" s="76"/>
+      <c r="O83" s="76"/>
+      <c r="P83" s="76"/>
+    </row>
+    <row r="84" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A84" s="80" t="s">
         <v>1009</v>
       </c>
-      <c r="B84" s="75"/>
-      <c r="C84" s="75"/>
-      <c r="D84" s="75"/>
-      <c r="E84" s="75"/>
-      <c r="F84" s="75"/>
-      <c r="G84" s="75"/>
-      <c r="H84" s="75"/>
-      <c r="I84" s="75"/>
-      <c r="J84" s="75"/>
-      <c r="K84" s="75"/>
-      <c r="L84" s="75"/>
-      <c r="M84" s="75"/>
-      <c r="N84" s="75"/>
-      <c r="O84" s="75"/>
-      <c r="P84" s="75"/>
-    </row>
-    <row r="85" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A85" s="93" t="s">
+      <c r="B84" s="76"/>
+      <c r="C84" s="76"/>
+      <c r="D84" s="76"/>
+      <c r="E84" s="76"/>
+      <c r="F84" s="76"/>
+      <c r="G84" s="76"/>
+      <c r="H84" s="76"/>
+      <c r="I84" s="76"/>
+      <c r="J84" s="76"/>
+      <c r="K84" s="76"/>
+      <c r="L84" s="76"/>
+      <c r="M84" s="76"/>
+      <c r="N84" s="76"/>
+      <c r="O84" s="76"/>
+      <c r="P84" s="76"/>
+    </row>
+    <row r="85" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A85" s="84" t="s">
         <v>1002</v>
       </c>
-      <c r="B85" s="75"/>
-      <c r="C85" s="75"/>
-      <c r="D85" s="75"/>
-      <c r="E85" s="75"/>
-      <c r="F85" s="75"/>
-      <c r="G85" s="75"/>
-      <c r="H85" s="75"/>
-      <c r="I85" s="75"/>
-      <c r="J85" s="75"/>
-      <c r="K85" s="75"/>
-      <c r="L85" s="75"/>
-      <c r="M85" s="75"/>
-      <c r="N85" s="75"/>
-      <c r="O85" s="75"/>
-      <c r="P85" s="75"/>
-    </row>
-    <row r="86" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A86" s="92" t="s">
+      <c r="B85" s="76"/>
+      <c r="C85" s="76"/>
+      <c r="D85" s="76"/>
+      <c r="E85" s="76"/>
+      <c r="F85" s="76"/>
+      <c r="G85" s="76"/>
+      <c r="H85" s="76"/>
+      <c r="I85" s="76"/>
+      <c r="J85" s="76"/>
+      <c r="K85" s="76"/>
+      <c r="L85" s="76"/>
+      <c r="M85" s="76"/>
+      <c r="N85" s="76"/>
+      <c r="O85" s="76"/>
+      <c r="P85" s="76"/>
+    </row>
+    <row r="86" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A86" s="86" t="s">
         <v>1010</v>
       </c>
-      <c r="B86" s="75"/>
-      <c r="C86" s="75"/>
-      <c r="D86" s="75"/>
-      <c r="E86" s="75"/>
-      <c r="F86" s="75"/>
-      <c r="G86" s="75"/>
-      <c r="H86" s="75"/>
-      <c r="I86" s="75"/>
-      <c r="J86" s="75"/>
-      <c r="K86" s="75"/>
-      <c r="L86" s="75"/>
-      <c r="M86" s="75"/>
-      <c r="N86" s="75"/>
-      <c r="O86" s="75"/>
-      <c r="P86" s="75"/>
-    </row>
-    <row r="87" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A87" s="93" t="s">
+      <c r="B86" s="76"/>
+      <c r="C86" s="76"/>
+      <c r="D86" s="76"/>
+      <c r="E86" s="76"/>
+      <c r="F86" s="76"/>
+      <c r="G86" s="76"/>
+      <c r="H86" s="76"/>
+      <c r="I86" s="76"/>
+      <c r="J86" s="76"/>
+      <c r="K86" s="76"/>
+      <c r="L86" s="76"/>
+      <c r="M86" s="76"/>
+      <c r="N86" s="76"/>
+      <c r="O86" s="76"/>
+      <c r="P86" s="76"/>
+    </row>
+    <row r="87" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A87" s="84" t="s">
         <v>1004</v>
       </c>
-      <c r="B87" s="75"/>
-      <c r="C87" s="75"/>
-      <c r="D87" s="75"/>
-      <c r="E87" s="75"/>
-      <c r="F87" s="75"/>
-      <c r="G87" s="75"/>
-      <c r="H87" s="75"/>
-      <c r="I87" s="75"/>
-      <c r="J87" s="75"/>
-      <c r="K87" s="75"/>
-      <c r="L87" s="75"/>
-      <c r="M87" s="75"/>
-      <c r="N87" s="75"/>
-      <c r="O87" s="75"/>
-      <c r="P87" s="75"/>
-    </row>
-    <row r="88" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A88" s="82" t="s">
+      <c r="B87" s="76"/>
+      <c r="C87" s="76"/>
+      <c r="D87" s="76"/>
+      <c r="E87" s="76"/>
+      <c r="F87" s="76"/>
+      <c r="G87" s="76"/>
+      <c r="H87" s="76"/>
+      <c r="I87" s="76"/>
+      <c r="J87" s="76"/>
+      <c r="K87" s="76"/>
+      <c r="L87" s="76"/>
+      <c r="M87" s="76"/>
+      <c r="N87" s="76"/>
+      <c r="O87" s="76"/>
+      <c r="P87" s="76"/>
+    </row>
+    <row r="88" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A88" s="83" t="s">
         <v>1011</v>
       </c>
-      <c r="B88" s="75"/>
-      <c r="C88" s="75"/>
-      <c r="D88" s="75"/>
-      <c r="E88" s="75"/>
-      <c r="F88" s="75"/>
-      <c r="G88" s="75"/>
-      <c r="H88" s="75"/>
-      <c r="I88" s="75"/>
-      <c r="J88" s="75"/>
-      <c r="K88" s="75"/>
-      <c r="L88" s="75"/>
-      <c r="M88" s="75"/>
-      <c r="N88" s="75"/>
-      <c r="O88" s="75"/>
-      <c r="P88" s="75"/>
-    </row>
-    <row r="89" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A89" s="77" t="s">
+      <c r="B88" s="76"/>
+      <c r="C88" s="76"/>
+      <c r="D88" s="76"/>
+      <c r="E88" s="76"/>
+      <c r="F88" s="76"/>
+      <c r="G88" s="76"/>
+      <c r="H88" s="76"/>
+      <c r="I88" s="76"/>
+      <c r="J88" s="76"/>
+      <c r="K88" s="76"/>
+      <c r="L88" s="76"/>
+      <c r="M88" s="76"/>
+      <c r="N88" s="76"/>
+      <c r="O88" s="76"/>
+      <c r="P88" s="76"/>
+    </row>
+    <row r="89" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A89" s="80" t="s">
         <v>1012</v>
       </c>
-      <c r="B89" s="75"/>
-      <c r="C89" s="75"/>
-      <c r="D89" s="75"/>
-      <c r="E89" s="75"/>
-      <c r="F89" s="75"/>
-      <c r="G89" s="75"/>
-      <c r="H89" s="75"/>
-      <c r="I89" s="75"/>
-      <c r="J89" s="75"/>
-      <c r="K89" s="75"/>
-      <c r="L89" s="75"/>
-      <c r="M89" s="75"/>
-      <c r="N89" s="75"/>
-      <c r="O89" s="75"/>
-      <c r="P89" s="75"/>
-    </row>
-    <row r="90" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A90" s="93" t="s">
+      <c r="B89" s="76"/>
+      <c r="C89" s="76"/>
+      <c r="D89" s="76"/>
+      <c r="E89" s="76"/>
+      <c r="F89" s="76"/>
+      <c r="G89" s="76"/>
+      <c r="H89" s="76"/>
+      <c r="I89" s="76"/>
+      <c r="J89" s="76"/>
+      <c r="K89" s="76"/>
+      <c r="L89" s="76"/>
+      <c r="M89" s="76"/>
+      <c r="N89" s="76"/>
+      <c r="O89" s="76"/>
+      <c r="P89" s="76"/>
+    </row>
+    <row r="90" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A90" s="84" t="s">
         <v>1007</v>
       </c>
-      <c r="B90" s="75"/>
-      <c r="C90" s="75"/>
-      <c r="D90" s="75"/>
-      <c r="E90" s="75"/>
-      <c r="F90" s="75"/>
-      <c r="G90" s="75"/>
-      <c r="H90" s="75"/>
-      <c r="I90" s="75"/>
-      <c r="J90" s="75"/>
-      <c r="K90" s="75"/>
-      <c r="L90" s="75"/>
-      <c r="M90" s="75"/>
-      <c r="N90" s="75"/>
-      <c r="O90" s="75"/>
-      <c r="P90" s="75"/>
-    </row>
-    <row r="91" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A91" s="80" t="s">
+      <c r="B90" s="76"/>
+      <c r="C90" s="76"/>
+      <c r="D90" s="76"/>
+      <c r="E90" s="76"/>
+      <c r="F90" s="76"/>
+      <c r="G90" s="76"/>
+      <c r="H90" s="76"/>
+      <c r="I90" s="76"/>
+      <c r="J90" s="76"/>
+      <c r="K90" s="76"/>
+      <c r="L90" s="76"/>
+      <c r="M90" s="76"/>
+      <c r="N90" s="76"/>
+      <c r="O90" s="76"/>
+      <c r="P90" s="76"/>
+    </row>
+    <row r="91" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A91" s="85" t="s">
         <v>1013</v>
       </c>
-      <c r="B91" s="75"/>
-      <c r="C91" s="75"/>
-      <c r="D91" s="75"/>
-      <c r="E91" s="75"/>
-      <c r="F91" s="75"/>
-      <c r="G91" s="75"/>
-      <c r="H91" s="75"/>
-      <c r="I91" s="75"/>
-      <c r="J91" s="75"/>
-      <c r="K91" s="75"/>
-      <c r="L91" s="75"/>
-      <c r="M91" s="75"/>
-      <c r="N91" s="75"/>
-      <c r="O91" s="75"/>
-      <c r="P91" s="75"/>
-    </row>
-    <row r="92" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A92" s="78" t="s">
+      <c r="B91" s="76"/>
+      <c r="C91" s="76"/>
+      <c r="D91" s="76"/>
+      <c r="E91" s="76"/>
+      <c r="F91" s="76"/>
+      <c r="G91" s="76"/>
+      <c r="H91" s="76"/>
+      <c r="I91" s="76"/>
+      <c r="J91" s="76"/>
+      <c r="K91" s="76"/>
+      <c r="L91" s="76"/>
+      <c r="M91" s="76"/>
+      <c r="N91" s="76"/>
+      <c r="O91" s="76"/>
+      <c r="P91" s="76"/>
+    </row>
+    <row r="92" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A92" s="79" t="s">
         <v>1014</v>
       </c>
-      <c r="B92" s="75"/>
-      <c r="C92" s="75"/>
-      <c r="D92" s="75"/>
-      <c r="E92" s="75"/>
-      <c r="F92" s="75"/>
-      <c r="G92" s="75"/>
-      <c r="H92" s="75"/>
-      <c r="I92" s="75"/>
-      <c r="J92" s="75"/>
-      <c r="K92" s="75"/>
-      <c r="L92" s="75"/>
-      <c r="M92" s="75"/>
-      <c r="N92" s="75"/>
-      <c r="O92" s="75"/>
-      <c r="P92" s="75"/>
-    </row>
-    <row r="93" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A93" s="78" t="s">
+      <c r="B92" s="76"/>
+      <c r="C92" s="76"/>
+      <c r="D92" s="76"/>
+      <c r="E92" s="76"/>
+      <c r="F92" s="76"/>
+      <c r="G92" s="76"/>
+      <c r="H92" s="76"/>
+      <c r="I92" s="76"/>
+      <c r="J92" s="76"/>
+      <c r="K92" s="76"/>
+      <c r="L92" s="76"/>
+      <c r="M92" s="76"/>
+      <c r="N92" s="76"/>
+      <c r="O92" s="76"/>
+      <c r="P92" s="76"/>
+    </row>
+    <row r="93" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A93" s="79" t="s">
         <v>1015</v>
       </c>
-      <c r="B93" s="75"/>
-      <c r="C93" s="75"/>
-      <c r="D93" s="75"/>
-      <c r="E93" s="75"/>
-      <c r="F93" s="75"/>
-      <c r="G93" s="75"/>
-      <c r="H93" s="75"/>
-      <c r="I93" s="75"/>
-      <c r="J93" s="75"/>
-      <c r="K93" s="75"/>
-      <c r="L93" s="75"/>
-      <c r="M93" s="75"/>
-      <c r="N93" s="75"/>
-      <c r="O93" s="75"/>
-      <c r="P93" s="75"/>
-    </row>
-    <row r="94" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A94" s="78" t="s">
+      <c r="B93" s="76"/>
+      <c r="C93" s="76"/>
+      <c r="D93" s="76"/>
+      <c r="E93" s="76"/>
+      <c r="F93" s="76"/>
+      <c r="G93" s="76"/>
+      <c r="H93" s="76"/>
+      <c r="I93" s="76"/>
+      <c r="J93" s="76"/>
+      <c r="K93" s="76"/>
+      <c r="L93" s="76"/>
+      <c r="M93" s="76"/>
+      <c r="N93" s="76"/>
+      <c r="O93" s="76"/>
+      <c r="P93" s="76"/>
+    </row>
+    <row r="94" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A94" s="79" t="s">
         <v>1016</v>
       </c>
-      <c r="B94" s="75"/>
-      <c r="C94" s="75"/>
-      <c r="D94" s="75"/>
-      <c r="E94" s="75"/>
-      <c r="F94" s="75"/>
-      <c r="G94" s="75"/>
-      <c r="H94" s="75"/>
-      <c r="I94" s="75"/>
-      <c r="J94" s="75"/>
-      <c r="K94" s="75"/>
-      <c r="L94" s="75"/>
-      <c r="M94" s="75"/>
-      <c r="N94" s="75"/>
-      <c r="O94" s="75"/>
-      <c r="P94" s="75"/>
-    </row>
-    <row r="95" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A95" s="80" t="s">
+      <c r="B94" s="76"/>
+      <c r="C94" s="76"/>
+      <c r="D94" s="76"/>
+      <c r="E94" s="76"/>
+      <c r="F94" s="76"/>
+      <c r="G94" s="76"/>
+      <c r="H94" s="76"/>
+      <c r="I94" s="76"/>
+      <c r="J94" s="76"/>
+      <c r="K94" s="76"/>
+      <c r="L94" s="76"/>
+      <c r="M94" s="76"/>
+      <c r="N94" s="76"/>
+      <c r="O94" s="76"/>
+      <c r="P94" s="76"/>
+    </row>
+    <row r="95" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A95" s="85" t="s">
         <v>1017</v>
       </c>
-      <c r="B95" s="75"/>
-      <c r="C95" s="75"/>
-      <c r="D95" s="75"/>
-      <c r="E95" s="75"/>
-      <c r="F95" s="75"/>
-      <c r="G95" s="75"/>
-      <c r="H95" s="75"/>
-      <c r="I95" s="75"/>
-      <c r="J95" s="75"/>
-      <c r="K95" s="75"/>
-      <c r="L95" s="75"/>
-      <c r="M95" s="75"/>
-      <c r="N95" s="75"/>
-      <c r="O95" s="75"/>
-      <c r="P95" s="75"/>
-    </row>
-    <row r="96" spans="1:16" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A96" s="78" t="s">
+      <c r="B95" s="76"/>
+      <c r="C95" s="76"/>
+      <c r="D95" s="76"/>
+      <c r="E95" s="76"/>
+      <c r="F95" s="76"/>
+      <c r="G95" s="76"/>
+      <c r="H95" s="76"/>
+      <c r="I95" s="76"/>
+      <c r="J95" s="76"/>
+      <c r="K95" s="76"/>
+      <c r="L95" s="76"/>
+      <c r="M95" s="76"/>
+      <c r="N95" s="76"/>
+      <c r="O95" s="76"/>
+      <c r="P95" s="76"/>
+    </row>
+    <row r="96" spans="1:16" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A96" s="79" t="s">
         <v>1018</v>
       </c>
-      <c r="B96" s="75"/>
-      <c r="C96" s="75"/>
-      <c r="D96" s="75"/>
-      <c r="E96" s="75"/>
-      <c r="F96" s="75"/>
-      <c r="G96" s="75"/>
-      <c r="H96" s="75"/>
-      <c r="I96" s="75"/>
-      <c r="J96" s="75"/>
-      <c r="K96" s="75"/>
-      <c r="L96" s="75"/>
-      <c r="M96" s="75"/>
-      <c r="N96" s="75"/>
-      <c r="O96" s="75"/>
-      <c r="P96" s="75"/>
-    </row>
-    <row r="97" spans="1:20" s="69" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A97" s="78" t="s">
+      <c r="B96" s="76"/>
+      <c r="C96" s="76"/>
+      <c r="D96" s="76"/>
+      <c r="E96" s="76"/>
+      <c r="F96" s="76"/>
+      <c r="G96" s="76"/>
+      <c r="H96" s="76"/>
+      <c r="I96" s="76"/>
+      <c r="J96" s="76"/>
+      <c r="K96" s="76"/>
+      <c r="L96" s="76"/>
+      <c r="M96" s="76"/>
+      <c r="N96" s="76"/>
+      <c r="O96" s="76"/>
+      <c r="P96" s="76"/>
+    </row>
+    <row r="97" spans="1:20" s="71" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A97" s="79" t="s">
         <v>1018</v>
       </c>
       <c r="B97" s="91"/>
@@ -84387,285 +84358,285 @@
       <c r="O97" s="91"/>
       <c r="P97" s="91"/>
     </row>
-    <row r="98" spans="1:20" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A98" s="80" t="s">
+    <row r="98" spans="1:20" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A98" s="85" t="s">
         <v>1019</v>
       </c>
-      <c r="B98" s="75"/>
-      <c r="C98" s="75"/>
-      <c r="D98" s="75"/>
-      <c r="E98" s="75"/>
-      <c r="F98" s="75"/>
-      <c r="G98" s="75"/>
-      <c r="H98" s="75"/>
-      <c r="I98" s="75"/>
-      <c r="J98" s="75"/>
-      <c r="K98" s="75"/>
-      <c r="L98" s="75"/>
-      <c r="M98" s="75"/>
-      <c r="N98" s="75"/>
-      <c r="O98" s="75"/>
-      <c r="P98" s="75"/>
-    </row>
-    <row r="99" spans="1:20" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A99" s="82" t="s">
+      <c r="B98" s="76"/>
+      <c r="C98" s="76"/>
+      <c r="D98" s="76"/>
+      <c r="E98" s="76"/>
+      <c r="F98" s="76"/>
+      <c r="G98" s="76"/>
+      <c r="H98" s="76"/>
+      <c r="I98" s="76"/>
+      <c r="J98" s="76"/>
+      <c r="K98" s="76"/>
+      <c r="L98" s="76"/>
+      <c r="M98" s="76"/>
+      <c r="N98" s="76"/>
+      <c r="O98" s="76"/>
+      <c r="P98" s="76"/>
+    </row>
+    <row r="99" spans="1:20" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A99" s="83" t="s">
         <v>1020</v>
       </c>
-      <c r="B99" s="75"/>
-      <c r="C99" s="75"/>
-      <c r="D99" s="75"/>
-      <c r="E99" s="75"/>
-      <c r="F99" s="75"/>
-      <c r="G99" s="75"/>
-      <c r="H99" s="75"/>
-      <c r="I99" s="75"/>
-      <c r="J99" s="75"/>
-      <c r="K99" s="75"/>
-      <c r="L99" s="75"/>
-      <c r="M99" s="75"/>
-      <c r="N99" s="75"/>
-      <c r="O99" s="75"/>
-      <c r="P99" s="75"/>
-    </row>
-    <row r="100" spans="1:20" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A100" s="78" t="s">
+      <c r="B99" s="76"/>
+      <c r="C99" s="76"/>
+      <c r="D99" s="76"/>
+      <c r="E99" s="76"/>
+      <c r="F99" s="76"/>
+      <c r="G99" s="76"/>
+      <c r="H99" s="76"/>
+      <c r="I99" s="76"/>
+      <c r="J99" s="76"/>
+      <c r="K99" s="76"/>
+      <c r="L99" s="76"/>
+      <c r="M99" s="76"/>
+      <c r="N99" s="76"/>
+      <c r="O99" s="76"/>
+      <c r="P99" s="76"/>
+    </row>
+    <row r="100" spans="1:20" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A100" s="79" t="s">
         <v>1021</v>
       </c>
-      <c r="B100" s="75"/>
-      <c r="C100" s="75"/>
-      <c r="D100" s="75"/>
-      <c r="E100" s="75"/>
-      <c r="F100" s="75"/>
-      <c r="G100" s="75"/>
-      <c r="H100" s="75"/>
-      <c r="I100" s="75"/>
-      <c r="J100" s="75"/>
-      <c r="K100" s="75"/>
-      <c r="L100" s="75"/>
-      <c r="M100" s="75"/>
-      <c r="N100" s="75"/>
-      <c r="O100" s="75"/>
-      <c r="P100" s="75"/>
-    </row>
-    <row r="101" spans="1:20" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A101" s="78" t="s">
+      <c r="B100" s="76"/>
+      <c r="C100" s="76"/>
+      <c r="D100" s="76"/>
+      <c r="E100" s="76"/>
+      <c r="F100" s="76"/>
+      <c r="G100" s="76"/>
+      <c r="H100" s="76"/>
+      <c r="I100" s="76"/>
+      <c r="J100" s="76"/>
+      <c r="K100" s="76"/>
+      <c r="L100" s="76"/>
+      <c r="M100" s="76"/>
+      <c r="N100" s="76"/>
+      <c r="O100" s="76"/>
+      <c r="P100" s="76"/>
+    </row>
+    <row r="101" spans="1:20" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A101" s="79" t="s">
         <v>1022</v>
       </c>
-      <c r="B101" s="75"/>
-      <c r="C101" s="75"/>
-      <c r="D101" s="75"/>
-      <c r="E101" s="75"/>
-      <c r="F101" s="75"/>
-      <c r="G101" s="75"/>
-      <c r="H101" s="75"/>
-      <c r="I101" s="75"/>
-      <c r="J101" s="75"/>
-      <c r="K101" s="75"/>
-      <c r="L101" s="75"/>
-      <c r="M101" s="75"/>
-      <c r="N101" s="75"/>
-      <c r="O101" s="75"/>
-      <c r="P101" s="75"/>
-    </row>
-    <row r="102" spans="1:20" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A102" s="78" t="s">
+      <c r="B101" s="76"/>
+      <c r="C101" s="76"/>
+      <c r="D101" s="76"/>
+      <c r="E101" s="76"/>
+      <c r="F101" s="76"/>
+      <c r="G101" s="76"/>
+      <c r="H101" s="76"/>
+      <c r="I101" s="76"/>
+      <c r="J101" s="76"/>
+      <c r="K101" s="76"/>
+      <c r="L101" s="76"/>
+      <c r="M101" s="76"/>
+      <c r="N101" s="76"/>
+      <c r="O101" s="76"/>
+      <c r="P101" s="76"/>
+    </row>
+    <row r="102" spans="1:20" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A102" s="79" t="s">
         <v>1023</v>
       </c>
-      <c r="B102" s="75"/>
-      <c r="C102" s="75"/>
-      <c r="D102" s="75"/>
-      <c r="E102" s="75"/>
-      <c r="F102" s="75"/>
-      <c r="G102" s="75"/>
-      <c r="H102" s="75"/>
-      <c r="I102" s="75"/>
-      <c r="J102" s="75"/>
-      <c r="K102" s="75"/>
-      <c r="L102" s="75"/>
-      <c r="M102" s="75"/>
-      <c r="N102" s="75"/>
-      <c r="O102" s="75"/>
-      <c r="P102" s="75"/>
-    </row>
-    <row r="103" spans="1:20" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A103" s="80" t="s">
+      <c r="B102" s="76"/>
+      <c r="C102" s="76"/>
+      <c r="D102" s="76"/>
+      <c r="E102" s="76"/>
+      <c r="F102" s="76"/>
+      <c r="G102" s="76"/>
+      <c r="H102" s="76"/>
+      <c r="I102" s="76"/>
+      <c r="J102" s="76"/>
+      <c r="K102" s="76"/>
+      <c r="L102" s="76"/>
+      <c r="M102" s="76"/>
+      <c r="N102" s="76"/>
+      <c r="O102" s="76"/>
+      <c r="P102" s="76"/>
+    </row>
+    <row r="103" spans="1:20" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A103" s="85" t="s">
         <v>1024</v>
       </c>
-      <c r="B103" s="75"/>
-      <c r="C103" s="75"/>
-      <c r="D103" s="75"/>
-      <c r="E103" s="75"/>
-      <c r="F103" s="75"/>
-      <c r="G103" s="75"/>
-      <c r="H103" s="75"/>
-      <c r="I103" s="75"/>
-      <c r="J103" s="75"/>
-      <c r="K103" s="75"/>
-      <c r="L103" s="75"/>
-      <c r="M103" s="75"/>
-      <c r="N103" s="75"/>
-      <c r="O103" s="75"/>
-      <c r="P103" s="75"/>
-    </row>
-    <row r="104" spans="1:20" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A104" s="82" t="s">
+      <c r="B103" s="76"/>
+      <c r="C103" s="76"/>
+      <c r="D103" s="76"/>
+      <c r="E103" s="76"/>
+      <c r="F103" s="76"/>
+      <c r="G103" s="76"/>
+      <c r="H103" s="76"/>
+      <c r="I103" s="76"/>
+      <c r="J103" s="76"/>
+      <c r="K103" s="76"/>
+      <c r="L103" s="76"/>
+      <c r="M103" s="76"/>
+      <c r="N103" s="76"/>
+      <c r="O103" s="76"/>
+      <c r="P103" s="76"/>
+    </row>
+    <row r="104" spans="1:20" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A104" s="83" t="s">
         <v>1025</v>
       </c>
-      <c r="B104" s="75"/>
-      <c r="C104" s="75"/>
-      <c r="D104" s="75"/>
-      <c r="E104" s="75"/>
-      <c r="F104" s="75"/>
-      <c r="G104" s="75"/>
-      <c r="H104" s="75"/>
-      <c r="I104" s="75"/>
-      <c r="J104" s="75"/>
-      <c r="K104" s="75"/>
-      <c r="L104" s="75"/>
-      <c r="M104" s="75"/>
-      <c r="N104" s="75"/>
-      <c r="O104" s="75"/>
-      <c r="P104" s="75"/>
-    </row>
-    <row r="105" spans="1:20" s="68" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A105" s="77" t="s">
+      <c r="B104" s="76"/>
+      <c r="C104" s="76"/>
+      <c r="D104" s="76"/>
+      <c r="E104" s="76"/>
+      <c r="F104" s="76"/>
+      <c r="G104" s="76"/>
+      <c r="H104" s="76"/>
+      <c r="I104" s="76"/>
+      <c r="J104" s="76"/>
+      <c r="K104" s="76"/>
+      <c r="L104" s="76"/>
+      <c r="M104" s="76"/>
+      <c r="N104" s="76"/>
+      <c r="O104" s="76"/>
+      <c r="P104" s="76"/>
+    </row>
+    <row r="105" spans="1:20" s="70" customFormat="1" ht="23.25" customHeight="1">
+      <c r="A105" s="80" t="s">
         <v>1026</v>
       </c>
-      <c r="B105" s="75"/>
-      <c r="C105" s="75"/>
-      <c r="D105" s="75"/>
-      <c r="E105" s="75"/>
-      <c r="F105" s="75"/>
-      <c r="G105" s="75"/>
-      <c r="H105" s="75"/>
-      <c r="I105" s="75"/>
-      <c r="J105" s="75"/>
-      <c r="K105" s="75"/>
-      <c r="L105" s="75"/>
-      <c r="M105" s="75"/>
-      <c r="N105" s="75"/>
-      <c r="O105" s="75"/>
-      <c r="P105" s="75"/>
-    </row>
-    <row r="106" spans="1:20" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A106" s="77" t="s">
+      <c r="B105" s="76"/>
+      <c r="C105" s="76"/>
+      <c r="D105" s="76"/>
+      <c r="E105" s="76"/>
+      <c r="F105" s="76"/>
+      <c r="G105" s="76"/>
+      <c r="H105" s="76"/>
+      <c r="I105" s="76"/>
+      <c r="J105" s="76"/>
+      <c r="K105" s="76"/>
+      <c r="L105" s="76"/>
+      <c r="M105" s="76"/>
+      <c r="N105" s="76"/>
+      <c r="O105" s="76"/>
+      <c r="P105" s="76"/>
+    </row>
+    <row r="106" spans="1:20" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A106" s="80" t="s">
         <v>1027</v>
       </c>
-      <c r="B106" s="75"/>
-      <c r="C106" s="75"/>
-      <c r="D106" s="75"/>
-      <c r="E106" s="75"/>
-      <c r="F106" s="75"/>
-      <c r="G106" s="75"/>
-      <c r="H106" s="75"/>
-      <c r="I106" s="75"/>
-      <c r="J106" s="75"/>
-      <c r="K106" s="75"/>
-      <c r="L106" s="75"/>
-      <c r="M106" s="75"/>
-      <c r="N106" s="75"/>
-      <c r="O106" s="75"/>
-      <c r="P106" s="75"/>
-    </row>
-    <row r="107" spans="1:20" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A107" s="82" t="s">
+      <c r="B106" s="76"/>
+      <c r="C106" s="76"/>
+      <c r="D106" s="76"/>
+      <c r="E106" s="76"/>
+      <c r="F106" s="76"/>
+      <c r="G106" s="76"/>
+      <c r="H106" s="76"/>
+      <c r="I106" s="76"/>
+      <c r="J106" s="76"/>
+      <c r="K106" s="76"/>
+      <c r="L106" s="76"/>
+      <c r="M106" s="76"/>
+      <c r="N106" s="76"/>
+      <c r="O106" s="76"/>
+      <c r="P106" s="76"/>
+    </row>
+    <row r="107" spans="1:20" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A107" s="83" t="s">
         <v>1028</v>
       </c>
-      <c r="B107" s="75"/>
-      <c r="C107" s="75"/>
-      <c r="D107" s="75"/>
-      <c r="E107" s="75"/>
-      <c r="F107" s="75"/>
-      <c r="G107" s="75"/>
-      <c r="H107" s="75"/>
-      <c r="I107" s="75"/>
-      <c r="J107" s="75"/>
-      <c r="K107" s="75"/>
-      <c r="L107" s="75"/>
-      <c r="M107" s="75"/>
-      <c r="N107" s="75"/>
-      <c r="O107" s="75"/>
-      <c r="P107" s="75"/>
-    </row>
-    <row r="108" spans="1:20" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A108" s="98" t="s">
+      <c r="B107" s="76"/>
+      <c r="C107" s="76"/>
+      <c r="D107" s="76"/>
+      <c r="E107" s="76"/>
+      <c r="F107" s="76"/>
+      <c r="G107" s="76"/>
+      <c r="H107" s="76"/>
+      <c r="I107" s="76"/>
+      <c r="J107" s="76"/>
+      <c r="K107" s="76"/>
+      <c r="L107" s="76"/>
+      <c r="M107" s="76"/>
+      <c r="N107" s="76"/>
+      <c r="O107" s="76"/>
+      <c r="P107" s="76"/>
+    </row>
+    <row r="108" spans="1:20" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A108" s="81" t="s">
         <v>1029</v>
       </c>
-      <c r="B108" s="75"/>
-      <c r="C108" s="75"/>
-      <c r="D108" s="75"/>
-      <c r="E108" s="75"/>
-      <c r="F108" s="75"/>
-      <c r="G108" s="75"/>
-      <c r="H108" s="75"/>
-      <c r="I108" s="75"/>
-      <c r="J108" s="75"/>
-      <c r="K108" s="75"/>
-      <c r="L108" s="75"/>
-      <c r="M108" s="75"/>
-      <c r="N108" s="75"/>
-      <c r="O108" s="75"/>
-      <c r="P108" s="75"/>
-    </row>
-    <row r="109" spans="1:20" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A109" s="99" t="s">
+      <c r="B108" s="76"/>
+      <c r="C108" s="76"/>
+      <c r="D108" s="76"/>
+      <c r="E108" s="76"/>
+      <c r="F108" s="76"/>
+      <c r="G108" s="76"/>
+      <c r="H108" s="76"/>
+      <c r="I108" s="76"/>
+      <c r="J108" s="76"/>
+      <c r="K108" s="76"/>
+      <c r="L108" s="76"/>
+      <c r="M108" s="76"/>
+      <c r="N108" s="76"/>
+      <c r="O108" s="76"/>
+      <c r="P108" s="76"/>
+    </row>
+    <row r="109" spans="1:20" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A109" s="82" t="s">
         <v>1030</v>
       </c>
-      <c r="B109" s="75"/>
-      <c r="C109" s="75"/>
-      <c r="D109" s="75"/>
-      <c r="E109" s="75"/>
-      <c r="F109" s="75"/>
-      <c r="G109" s="75"/>
-      <c r="H109" s="75"/>
-      <c r="I109" s="75"/>
-      <c r="J109" s="75"/>
-      <c r="K109" s="75"/>
-      <c r="L109" s="75"/>
-      <c r="M109" s="75"/>
-      <c r="N109" s="75"/>
-      <c r="O109" s="75"/>
-      <c r="P109" s="75"/>
-    </row>
-    <row r="110" spans="1:20" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A110" s="82" t="s">
+      <c r="B109" s="76"/>
+      <c r="C109" s="76"/>
+      <c r="D109" s="76"/>
+      <c r="E109" s="76"/>
+      <c r="F109" s="76"/>
+      <c r="G109" s="76"/>
+      <c r="H109" s="76"/>
+      <c r="I109" s="76"/>
+      <c r="J109" s="76"/>
+      <c r="K109" s="76"/>
+      <c r="L109" s="76"/>
+      <c r="M109" s="76"/>
+      <c r="N109" s="76"/>
+      <c r="O109" s="76"/>
+      <c r="P109" s="76"/>
+    </row>
+    <row r="110" spans="1:20" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A110" s="83" t="s">
         <v>1031</v>
       </c>
-      <c r="B110" s="75"/>
-      <c r="C110" s="75"/>
-      <c r="D110" s="75"/>
-      <c r="E110" s="75"/>
-      <c r="F110" s="75"/>
-      <c r="G110" s="75"/>
-      <c r="H110" s="75"/>
-      <c r="I110" s="75"/>
-      <c r="J110" s="75"/>
-      <c r="K110" s="75"/>
-      <c r="L110" s="75"/>
-      <c r="M110" s="75"/>
-      <c r="N110" s="75"/>
-      <c r="O110" s="75"/>
-      <c r="P110" s="75"/>
-    </row>
-    <row r="111" spans="1:20" s="68" customFormat="1" ht="12.75" customHeight="1">
-      <c r="A111" s="78" t="s">
+      <c r="B110" s="76"/>
+      <c r="C110" s="76"/>
+      <c r="D110" s="76"/>
+      <c r="E110" s="76"/>
+      <c r="F110" s="76"/>
+      <c r="G110" s="76"/>
+      <c r="H110" s="76"/>
+      <c r="I110" s="76"/>
+      <c r="J110" s="76"/>
+      <c r="K110" s="76"/>
+      <c r="L110" s="76"/>
+      <c r="M110" s="76"/>
+      <c r="N110" s="76"/>
+      <c r="O110" s="76"/>
+      <c r="P110" s="76"/>
+    </row>
+    <row r="111" spans="1:20" s="70" customFormat="1" ht="12.75" customHeight="1">
+      <c r="A111" s="79" t="s">
         <v>1032</v>
       </c>
-      <c r="B111" s="75"/>
-      <c r="C111" s="75"/>
-      <c r="D111" s="75"/>
-      <c r="E111" s="75"/>
-      <c r="F111" s="75"/>
-      <c r="G111" s="75"/>
-      <c r="H111" s="75"/>
-      <c r="I111" s="75"/>
-      <c r="J111" s="75"/>
-      <c r="K111" s="75"/>
-      <c r="L111" s="75"/>
-      <c r="M111" s="75"/>
-      <c r="N111" s="75"/>
-      <c r="O111" s="75"/>
-      <c r="P111" s="75"/>
+      <c r="B111" s="76"/>
+      <c r="C111" s="76"/>
+      <c r="D111" s="76"/>
+      <c r="E111" s="76"/>
+      <c r="F111" s="76"/>
+      <c r="G111" s="76"/>
+      <c r="H111" s="76"/>
+      <c r="I111" s="76"/>
+      <c r="J111" s="76"/>
+      <c r="K111" s="76"/>
+      <c r="L111" s="76"/>
+      <c r="M111" s="76"/>
+      <c r="N111" s="76"/>
+      <c r="O111" s="76"/>
+      <c r="P111" s="76"/>
     </row>
     <row r="112" spans="1:20" s="23" customFormat="1" ht="12.75" customHeight="1">
       <c r="A112" s="55"/>
@@ -84685,38 +84656,38 @@
       <c r="O112" s="22"/>
       <c r="T112" s="24"/>
     </row>
-    <row r="113" spans="1:20" s="25" customFormat="1" ht="11.1" customHeight="1">
+    <row r="113" spans="1:20" s="25" customFormat="1" ht="11" customHeight="1">
       <c r="T113" s="26"/>
     </row>
-    <row r="114" spans="1:20" s="25" customFormat="1" ht="13.5">
+    <row r="114" spans="1:20" s="25" customFormat="1" ht="13.5" customHeight="1">
       <c r="A114" s="38"/>
       <c r="T114" s="26"/>
     </row>
-    <row r="115" spans="1:20" s="25" customFormat="1" ht="13.5">
+    <row r="115" spans="1:20" s="25" customFormat="1" ht="13.5" customHeight="1">
       <c r="A115" s="38"/>
       <c r="T115" s="26"/>
     </row>
-    <row r="116" spans="1:20" s="25" customFormat="1" ht="13.5">
+    <row r="116" spans="1:20" s="25" customFormat="1" ht="13.5" customHeight="1">
       <c r="A116" s="38"/>
       <c r="T116" s="26"/>
     </row>
-    <row r="117" spans="1:20" s="25" customFormat="1" ht="13.5">
+    <row r="117" spans="1:20" s="25" customFormat="1" ht="13.5" customHeight="1">
       <c r="A117" s="38"/>
       <c r="T117" s="26"/>
     </row>
-    <row r="118" spans="1:20" s="25" customFormat="1" ht="13.5">
+    <row r="118" spans="1:20" s="25" customFormat="1" ht="13.5" customHeight="1">
       <c r="A118" s="38"/>
       <c r="T118" s="26"/>
     </row>
-    <row r="119" spans="1:20" s="25" customFormat="1" ht="13.5">
+    <row r="119" spans="1:20" s="25" customFormat="1" ht="13.5" customHeight="1">
       <c r="A119" s="38"/>
       <c r="T119" s="26"/>
     </row>
-    <row r="120" spans="1:20" s="25" customFormat="1" ht="13.5">
+    <row r="120" spans="1:20" s="25" customFormat="1" ht="13.5" customHeight="1">
       <c r="A120" s="38"/>
       <c r="T120" s="26"/>
     </row>
-    <row r="121" spans="1:20" s="25" customFormat="1" ht="13.5">
+    <row r="121" spans="1:20" s="25" customFormat="1" ht="13.5" customHeight="1">
       <c r="A121" s="38"/>
       <c r="B121" s="38"/>
       <c r="C121" s="38"/>
@@ -84725,15 +84696,59 @@
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="A46:R46"/>
-    <mergeCell ref="A47:R47"/>
-    <mergeCell ref="A48:R48"/>
-    <mergeCell ref="A49:R49"/>
-    <mergeCell ref="A41:R41"/>
-    <mergeCell ref="A42:R42"/>
-    <mergeCell ref="A43:R43"/>
-    <mergeCell ref="A44:R44"/>
-    <mergeCell ref="A45:R45"/>
+    <mergeCell ref="A39:R39"/>
+    <mergeCell ref="A51:P51"/>
+    <mergeCell ref="A76:P76"/>
+    <mergeCell ref="A70:P70"/>
+    <mergeCell ref="A65:P65"/>
+    <mergeCell ref="A55:P55"/>
+    <mergeCell ref="A56:P56"/>
+    <mergeCell ref="A57:P57"/>
+    <mergeCell ref="A71:P71"/>
+    <mergeCell ref="A72:P72"/>
+    <mergeCell ref="A73:P73"/>
+    <mergeCell ref="A74:P74"/>
+    <mergeCell ref="A69:P69"/>
+    <mergeCell ref="A59:P59"/>
+    <mergeCell ref="A75:P75"/>
+    <mergeCell ref="A40:R40"/>
+    <mergeCell ref="A1:AI1"/>
+    <mergeCell ref="A35:R35"/>
+    <mergeCell ref="A36:R36"/>
+    <mergeCell ref="A37:R37"/>
+    <mergeCell ref="A38:R38"/>
+    <mergeCell ref="A107:P107"/>
+    <mergeCell ref="A100:P100"/>
+    <mergeCell ref="A97:P97"/>
+    <mergeCell ref="A99:P99"/>
+    <mergeCell ref="A96:P96"/>
+    <mergeCell ref="A98:P98"/>
+    <mergeCell ref="A101:P101"/>
+    <mergeCell ref="A78:P78"/>
+    <mergeCell ref="A79:P79"/>
+    <mergeCell ref="A80:P80"/>
+    <mergeCell ref="A52:P52"/>
+    <mergeCell ref="A53:P53"/>
+    <mergeCell ref="A58:P58"/>
+    <mergeCell ref="A54:P54"/>
+    <mergeCell ref="A77:P77"/>
+    <mergeCell ref="A60:P60"/>
+    <mergeCell ref="A61:P61"/>
+    <mergeCell ref="A62:P62"/>
+    <mergeCell ref="A63:P63"/>
+    <mergeCell ref="A64:P64"/>
+    <mergeCell ref="A66:P66"/>
+    <mergeCell ref="A67:P67"/>
+    <mergeCell ref="A68:P68"/>
+    <mergeCell ref="A89:P89"/>
+    <mergeCell ref="A90:P90"/>
+    <mergeCell ref="A95:P95"/>
+    <mergeCell ref="A81:P81"/>
+    <mergeCell ref="A82:P82"/>
+    <mergeCell ref="A84:P84"/>
+    <mergeCell ref="A85:P85"/>
+    <mergeCell ref="A86:P86"/>
+    <mergeCell ref="A83:P83"/>
     <mergeCell ref="A111:P111"/>
     <mergeCell ref="A50:P50"/>
     <mergeCell ref="A92:P92"/>
@@ -84750,59 +84765,15 @@
     <mergeCell ref="A103:P103"/>
     <mergeCell ref="A104:P104"/>
     <mergeCell ref="A91:P91"/>
-    <mergeCell ref="A89:P89"/>
-    <mergeCell ref="A90:P90"/>
-    <mergeCell ref="A95:P95"/>
-    <mergeCell ref="A81:P81"/>
-    <mergeCell ref="A82:P82"/>
-    <mergeCell ref="A84:P84"/>
-    <mergeCell ref="A85:P85"/>
-    <mergeCell ref="A86:P86"/>
-    <mergeCell ref="A83:P83"/>
-    <mergeCell ref="A78:P78"/>
-    <mergeCell ref="A79:P79"/>
-    <mergeCell ref="A80:P80"/>
-    <mergeCell ref="A52:P52"/>
-    <mergeCell ref="A53:P53"/>
-    <mergeCell ref="A58:P58"/>
-    <mergeCell ref="A54:P54"/>
-    <mergeCell ref="A77:P77"/>
-    <mergeCell ref="A60:P60"/>
-    <mergeCell ref="A61:P61"/>
-    <mergeCell ref="A62:P62"/>
-    <mergeCell ref="A63:P63"/>
-    <mergeCell ref="A64:P64"/>
-    <mergeCell ref="A66:P66"/>
-    <mergeCell ref="A67:P67"/>
-    <mergeCell ref="A68:P68"/>
-    <mergeCell ref="A107:P107"/>
-    <mergeCell ref="A100:P100"/>
-    <mergeCell ref="A97:P97"/>
-    <mergeCell ref="A99:P99"/>
-    <mergeCell ref="A96:P96"/>
-    <mergeCell ref="A98:P98"/>
-    <mergeCell ref="A101:P101"/>
-    <mergeCell ref="A1:AI1"/>
-    <mergeCell ref="A35:R35"/>
-    <mergeCell ref="A36:R36"/>
-    <mergeCell ref="A37:R37"/>
-    <mergeCell ref="A38:R38"/>
-    <mergeCell ref="A39:R39"/>
-    <mergeCell ref="A51:P51"/>
-    <mergeCell ref="A76:P76"/>
-    <mergeCell ref="A70:P70"/>
-    <mergeCell ref="A65:P65"/>
-    <mergeCell ref="A55:P55"/>
-    <mergeCell ref="A56:P56"/>
-    <mergeCell ref="A57:P57"/>
-    <mergeCell ref="A71:P71"/>
-    <mergeCell ref="A72:P72"/>
-    <mergeCell ref="A73:P73"/>
-    <mergeCell ref="A74:P74"/>
-    <mergeCell ref="A69:P69"/>
-    <mergeCell ref="A59:P59"/>
-    <mergeCell ref="A75:P75"/>
-    <mergeCell ref="A40:R40"/>
+    <mergeCell ref="A46:R46"/>
+    <mergeCell ref="A47:R47"/>
+    <mergeCell ref="A48:R48"/>
+    <mergeCell ref="A49:R49"/>
+    <mergeCell ref="A41:R41"/>
+    <mergeCell ref="A42:R42"/>
+    <mergeCell ref="A43:R43"/>
+    <mergeCell ref="A44:R44"/>
+    <mergeCell ref="A45:R45"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="35" fitToHeight="0" orientation="landscape"/>

</xml_diff>